<commit_message>
add more papers for adipocyte size
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51937E55-2A16-E442-A5AD-9436CF7AD20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370710E4-DC56-E046-9AA1-6E93BF8D1B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="740" windowWidth="22400" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -506,20 +506,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Lijnen2006</t>
   </si>
   <si>
-    <t>Lijnen2001</t>
-  </si>
-  <si>
-    <t>Maquoi2002</t>
-  </si>
-  <si>
-    <t>Morange2000</t>
-  </si>
-  <si>
     <t>Voros2005</t>
   </si>
   <si>
@@ -572,6 +563,36 @@
   </si>
   <si>
     <t>Obese SD</t>
+  </si>
+  <si>
+    <t>Lijnen et al., 2006</t>
+  </si>
+  <si>
+    <t>Lijnen et al., 2001</t>
+  </si>
+  <si>
+    <t>Maquoi et al., 2002</t>
+  </si>
+  <si>
+    <t>Morange et al.,2000</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005</t>
+  </si>
+  <si>
+    <t>Lijnen, Maquoi et al., 2003</t>
+  </si>
+  <si>
+    <t>Lijnen et al., 2003</t>
+  </si>
+  <si>
+    <t>Maquoi et al., 2003</t>
+  </si>
+  <si>
+    <t>Lijnen et al., 2007</t>
+  </si>
+  <si>
+    <t>Van Hul et al., 2012</t>
   </si>
 </sst>
 </file>
@@ -794,7 +815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -805,17 +826,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -828,6 +840,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,51 +1173,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C9A479-2AA3-884B-8FF7-FA729F57839B}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>12</v>
+      <c r="A1" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
+      <c r="A2" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="B2" s="2">
         <v>44.993898209967412</v>
@@ -1200,14 +1228,14 @@
       <c r="D2" s="2">
         <v>65.795246424795408</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>1.838396591281048</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1">
         <v>1590</v>
@@ -1223,8 +1251,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>1</v>
+      <c r="A3" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="B3" s="1">
         <v>49</v>
@@ -1235,12 +1263,12 @@
       <c r="D3" s="1">
         <v>80</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>5.3</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="16"/>
       <c r="H3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I3" s="1">
         <f>SQRT(I2/PI())</f>
@@ -1260,8 +1288,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>2</v>
+      <c r="A4" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>42</v>
@@ -1270,12 +1298,12 @@
       <c r="D4" s="1">
         <v>83</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="19"/>
+      <c r="G4" s="16"/>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1">
         <f>I3*2</f>
@@ -1295,8 +1323,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>3</v>
+      <c r="A5" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>49</v>
@@ -1307,14 +1335,14 @@
       <c r="D5" s="1">
         <v>82</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>3.5</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>4</v>
+      <c r="G5" s="16" t="s">
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I5" s="1">
         <v>650</v>
@@ -1329,25 +1357,25 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1">
         <v>28.76813695875796</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="1">
         <v>1.0622081338618323</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="1">
         <v>52.925674284012274</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="7">
         <v>0.45708536881646961</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1">
         <f>SQRT(I5/PI())</f>
@@ -1367,9 +1395,24 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G7" s="19"/>
+      <c r="A7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="19">
+        <v>62</v>
+      </c>
+      <c r="C7" s="19">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D7" s="19">
+        <v>85</v>
+      </c>
+      <c r="E7" s="21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G7" s="16"/>
       <c r="H7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1">
         <f>I6*2</f>
@@ -1388,9 +1431,67 @@
         <v>0.45708536881646961</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="19">
+        <v>40.049999999999997</v>
+      </c>
+      <c r="C8" s="19">
+        <v>0.76</v>
+      </c>
+      <c r="D8" s="19">
+        <v>94.61</v>
+      </c>
+      <c r="E8" s="21">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="19">
+        <v>76.36</v>
+      </c>
+      <c r="E9" s="21">
+        <v>2.25</v>
+      </c>
+    </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="19">
+        <v>89.13</v>
+      </c>
+      <c r="E10" s="21">
+        <v>1.46</v>
+      </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="8">
+        <v>42.4</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1.95</v>
+      </c>
+      <c r="D11" s="20">
+        <v>58.37</v>
+      </c>
+      <c r="E11" s="22">
+        <v>2.2200000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1427,7 +1528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1440,24 +1541,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>16</v>
+      <c r="A2" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="2">
         <v>69</v>
@@ -1466,11 +1567,11 @@
         <v>5.5</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>15</v>
+      <c r="A3" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>56.78</v>
@@ -1479,11 +1580,11 @@
         <v>12.5</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>17</v>
+      <c r="A4" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>73</v>
@@ -1492,11 +1593,11 @@
         <v>16</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>18</v>
+      <c r="A5" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>92.87</v>
@@ -1505,11 +1606,11 @@
         <v>18.899999999999999</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>18</v>
+      <c r="A6" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>76.75</v>
@@ -1518,11 +1619,11 @@
         <v>14.17</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>13</v>
+      <c r="A7" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>62</v>
@@ -1534,14 +1635,14 @@
       <c r="D7" s="1">
         <v>68</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <f>12.1/1.96*SQRT(4)</f>
         <v>12.346938775510203</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>13</v>
+      <c r="A8" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>56</v>
@@ -1553,26 +1654,26 @@
       <c r="D8" s="1">
         <v>58</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <f>6.57/1.96*SQRT(5)</f>
         <v>7.4953911286600103</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="11">
+      <c r="A9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="8">
         <v>89</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
         <f>B9*2.2/100*2</f>
         <v>3.9160000000000004</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>113.4</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="9">
         <f>B9*2/100*2</f>
         <v>3.56</v>
       </c>

</xml_diff>

<commit_message>
edit reference notation in CBM thickness
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370710E4-DC56-E046-9AA1-6E93BF8D1B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62C9B77-67E5-B541-BFD1-CF100E45F0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -506,7 +506,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -538,24 +538,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Lash1989</t>
-  </si>
-  <si>
-    <t>Danis1993</t>
-  </si>
-  <si>
-    <t>Ceafalan2019</t>
-  </si>
-  <si>
-    <t>Rodrigues1983</t>
-  </si>
-  <si>
-    <t>Creutzfeldt</t>
-  </si>
-  <si>
-    <t>Calson2003</t>
-  </si>
-  <si>
     <t>dr = r/(2A)*dA</t>
   </si>
   <si>
@@ -593,6 +575,30 @@
   </si>
   <si>
     <t>Van Hul et al., 2012</t>
+  </si>
+  <si>
+    <t>Rodrigues et al., 1983</t>
+  </si>
+  <si>
+    <t>Ceafalan et al., 2019</t>
+  </si>
+  <si>
+    <t>Creutzfeldt et al., 1970</t>
+  </si>
+  <si>
+    <t>Calson et al., 2003 (muscle)</t>
+  </si>
+  <si>
+    <t>Calson et al., 2003 (retina)</t>
+  </si>
+  <si>
+    <t>Lash et al., 1989 (11 wk.)</t>
+  </si>
+  <si>
+    <t>Lash et al., 1989 (18 wk.)</t>
+  </si>
+  <si>
+    <t>Danis &amp; Yang, 1993</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1223,7 @@
     </row>
     <row r="2" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2">
         <v>44.993898209967412</v>
@@ -1252,7 +1258,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>49</v>
@@ -1289,7 +1295,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>42</v>
@@ -1324,7 +1330,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>49</v>
@@ -1359,7 +1365,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
         <v>28.76813695875796</v>
@@ -1396,7 +1402,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" s="19">
         <v>62</v>
@@ -1433,7 +1439,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" s="19">
         <v>40.049999999999997</v>
@@ -1450,7 +1456,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1463,7 +1469,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1474,12 +1480,12 @@
         <v>1.46</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B11" s="8">
         <v>42.4</v>
@@ -1529,12 +1535,12 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1547,18 +1553,18 @@
         <v>2</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2">
         <v>69</v>
@@ -1571,7 +1577,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
         <v>56.78</v>
@@ -1584,7 +1590,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1">
         <v>73</v>
@@ -1597,7 +1603,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1">
         <v>92.87</v>
@@ -1610,7 +1616,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1">
         <v>76.75</v>
@@ -1623,7 +1629,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
         <v>62</v>
@@ -1642,7 +1648,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
         <v>56</v>
@@ -1661,7 +1667,7 @@
     </row>
     <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B9" s="8">
         <v>89</v>

</xml_diff>

<commit_message>
add number of samples and calculate SE to the CBM thickness sheet
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62C9B77-67E5-B541-BFD1-CF100E45F0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8416A6-1FC7-2B43-9A35-DB54B1E3BCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -294,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{7E6B9E3B-D048-FF44-B063-87A613674E19}">
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{7E6B9E3B-D048-FF44-B063-87A613674E19}">
       <text>
         <r>
           <rPr>
@@ -351,7 +351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{D0891471-D081-7D49-A638-FDD2E6BE6EA6}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{D0891471-D081-7D49-A638-FDD2E6BE6EA6}">
       <text>
         <r>
           <rPr>
@@ -448,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
       <text>
         <r>
           <rPr>
@@ -506,7 +506,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -599,6 +599,12 @@
   </si>
   <si>
     <t>Danis &amp; Yang, 1993</t>
+  </si>
+  <si>
+    <t>Lean N</t>
+  </si>
+  <si>
+    <t>Obese N</t>
   </si>
 </sst>
 </file>
@@ -635,7 +641,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -817,11 +823,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -843,7 +929,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -863,6 +948,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1222,7 +1313,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2">
@@ -1237,7 +1328,7 @@
       <c r="E2" s="6">
         <v>1.838396591281048</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1257,7 +1348,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1">
@@ -1272,7 +1363,7 @@
       <c r="E3" s="7">
         <v>5.3</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1294,7 +1385,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="1">
@@ -1307,7 +1398,7 @@
       <c r="E4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1329,7 +1420,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1">
@@ -1344,7 +1435,7 @@
       <c r="E5" s="7">
         <v>3.5</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1364,7 +1455,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="1">
@@ -1379,7 +1470,7 @@
       <c r="E6" s="7">
         <v>0.45708536881646961</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1401,22 +1492,22 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>62</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="18">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="18">
         <v>85</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G7" s="16"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1438,45 +1529,45 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>40.049999999999997</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="18">
         <v>0.76</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>94.61</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>4.58</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <v>76.36</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="20">
         <v>2.25</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <v>89.13</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <v>1.46</v>
       </c>
       <c r="I10" t="s">
@@ -1484,7 +1575,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="8">
@@ -1493,10 +1584,10 @@
       <c r="C11" s="8">
         <v>1.95</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="19">
         <v>58.37</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="21">
         <v>2.2200000000000002</v>
       </c>
     </row>
@@ -1532,20 +1623,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1556,13 +1647,25 @@
         <v>11</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="G1" s="24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
@@ -1573,9 +1676,13 @@
         <v>5.5</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
@@ -1585,10 +1692,19 @@
       <c r="C3" s="1">
         <v>12.5</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="2">
+        <v>100</v>
+      </c>
+      <c r="E3" s="2">
+        <f>C3/SQRT(D3)</f>
+        <v>1.25</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
@@ -1598,10 +1714,19 @@
       <c r="C4" s="1">
         <v>16</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
+        <f>C4/SQRT(D4)</f>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>27</v>
       </c>
@@ -1611,10 +1736,19 @@
       <c r="C5" s="1">
         <v>18.899999999999999</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E8" si="0">C5/SQRT(D5)</f>
+        <v>6.6821590822128734</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
@@ -1624,10 +1758,19 @@
       <c r="C6" s="1">
         <v>14.17</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="2">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4809474444585931</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>28</v>
       </c>
@@ -1635,18 +1778,32 @@
         <v>62</v>
       </c>
       <c r="C7" s="1">
-        <f>6.64/1.96*SQRT(4)</f>
-        <v>6.7755102040816322</v>
+        <f>6.64/1.96*SQRT(6)</f>
+        <v>8.2982713735103566</v>
       </c>
       <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>3.3877551020408156</v>
+      </c>
+      <c r="F7" s="1">
         <v>68</v>
       </c>
-      <c r="E7" s="7">
-        <f>12.1/1.96*SQRT(4)</f>
-        <v>12.346938775510203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" s="26">
+        <f>12.1/1.96*SQRT(6)</f>
+        <v>15.121849942692066</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6</v>
+      </c>
+      <c r="I7" s="7">
+        <f>G7/SQRT(H7)</f>
+        <v>6.1734693877551017</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>29</v>
       </c>
@@ -1654,34 +1811,52 @@
         <v>56</v>
       </c>
       <c r="C8" s="1">
-        <f>7.32/1.96*SQRT(3)</f>
-        <v>6.4686795466347871</v>
+        <f>7.32/1.96*SQRT(6)</f>
+        <v>9.148094345496359</v>
       </c>
       <c r="D8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>3.7346938775510208</v>
+      </c>
+      <c r="F8" s="1">
         <v>58</v>
       </c>
-      <c r="E8" s="7">
-        <f>6.57/1.96*SQRT(5)</f>
-        <v>7.4953911286600103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="26">
+        <f>6.57/1.96*SQRT(7)</f>
+        <v>8.8686663845379403</v>
+      </c>
+      <c r="H8" s="1">
+        <v>7</v>
+      </c>
+      <c r="I8" s="7">
+        <f>G8/SQRT(H8)</f>
+        <v>3.3520408163265309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="8">
         <v>89</v>
       </c>
-      <c r="C9" s="8">
-        <f>B9*2.2/100*2</f>
-        <v>3.9160000000000004</v>
-      </c>
-      <c r="D9" s="8">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8">
+        <f>B9*2.2/100</f>
+        <v>1.9580000000000002</v>
+      </c>
+      <c r="F9" s="8">
         <v>113.4</v>
       </c>
-      <c r="E9" s="9">
-        <f>B9*2/100*2</f>
-        <v>3.56</v>
+      <c r="G9" s="27"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9">
+        <f>B9*2/100</f>
+        <v>1.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit standard error of CBM thickness in (Lash, 1989)
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8416A6-1FC7-2B43-9A35-DB54B1E3BCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F45D40-CFD5-B742-943B-F1D7D8CA4586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -267,121 +267,6 @@
             <family val="2"/>
           </rPr>
           <t>SD = 14.17</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{2A46D8DF-C71C-DB4B-97D6-6C1414099FF0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Yunjeong Lee:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Calculated from 95% CI of total wall thickness and endothelial cell thickness (n=4)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{7E6B9E3B-D048-FF44-B063-87A613674E19}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yunjeong Lee:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Calculated from 95% CI of total wall thickness and endothelial cell thickness (n=4)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{632CA213-3BB7-0745-AF20-0BE8597213A8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Yunjeong Lee:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Calculated from 95% CI of total wall thickness and endothelial cell thickness (n=3)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{D0891471-D081-7D49-A638-FDD2E6BE6EA6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yunjeong Lee:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Calculated from 95% CI of total wall thickness and endothelial cell thickness (n=5)
-</t>
         </r>
       </text>
     </comment>
@@ -907,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -929,31 +814,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,7 +1191,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2">
@@ -1328,7 +1206,7 @@
       <c r="E2" s="6">
         <v>1.838396591281048</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="24" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1348,7 +1226,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1">
@@ -1363,7 +1241,7 @@
       <c r="E3" s="7">
         <v>5.3</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1385,7 +1263,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="1">
@@ -1398,7 +1276,7 @@
       <c r="E4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1420,7 +1298,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1">
@@ -1435,7 +1313,7 @@
       <c r="E5" s="7">
         <v>3.5</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="24" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1455,7 +1333,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="1">
@@ -1470,7 +1348,7 @@
       <c r="E6" s="7">
         <v>0.45708536881646961</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1492,22 +1370,22 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="1">
         <v>62</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="1">
         <v>85</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1529,45 +1407,45 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="1">
         <v>40.049999999999997</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="1">
         <v>0.76</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="1">
         <v>94.61</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="7">
         <v>4.58</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="18">
+      <c r="D9" s="1">
         <v>76.36</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="7">
         <v>2.25</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="18">
+      <c r="D10" s="1">
         <v>89.13</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="7">
         <v>1.46</v>
       </c>
       <c r="I10" t="s">
@@ -1575,7 +1453,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="8">
@@ -1584,10 +1462,10 @@
       <c r="C11" s="8">
         <v>1.95</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="8">
         <v>58.37</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="9">
         <v>2.2200000000000002</v>
       </c>
     </row>
@@ -1626,7 +1504,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1655,13 +1533,13 @@
       <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1678,7 +1556,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="25"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="2"/>
       <c r="I2" s="6"/>
     </row>
@@ -1700,7 +1578,7 @@
         <v>1.25</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="25"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="1"/>
       <c r="I3" s="7"/>
     </row>
@@ -1722,7 +1600,7 @@
         <v>5.6568542494923797</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="25"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="1"/>
       <c r="I4" s="7"/>
     </row>
@@ -1744,7 +1622,7 @@
         <v>6.6821590822128734</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="25"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="1"/>
       <c r="I5" s="7"/>
     </row>
@@ -1766,7 +1644,7 @@
         <v>4.4809474444585931</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="25"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="1"/>
       <c r="I6" s="7"/>
     </row>
@@ -1775,32 +1653,24 @@
         <v>28</v>
       </c>
       <c r="B7" s="1">
-        <v>62</v>
-      </c>
-      <c r="C7" s="1">
-        <f>6.64/1.96*SQRT(6)</f>
-        <v>8.2982713735103566</v>
-      </c>
+        <v>61.87</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>6</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>3.3877551020408156</v>
+        <v>1.33</v>
       </c>
       <c r="F7" s="1">
-        <v>68</v>
-      </c>
-      <c r="G7" s="26">
-        <f>12.1/1.96*SQRT(6)</f>
-        <v>15.121849942692066</v>
-      </c>
+        <v>68.13</v>
+      </c>
+      <c r="G7" s="20"/>
       <c r="H7" s="1">
         <v>6</v>
       </c>
       <c r="I7" s="7">
-        <f>G7/SQRT(H7)</f>
-        <v>6.1734693877551017</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1808,32 +1678,24 @@
         <v>29</v>
       </c>
       <c r="B8" s="1">
-        <v>56</v>
-      </c>
-      <c r="C8" s="1">
-        <f>7.32/1.96*SQRT(6)</f>
-        <v>9.148094345496359</v>
-      </c>
+        <v>55.67</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1">
         <v>6</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>3.7346938775510208</v>
+        <v>1.04</v>
       </c>
       <c r="F8" s="1">
-        <v>58</v>
-      </c>
-      <c r="G8" s="26">
-        <f>6.57/1.96*SQRT(7)</f>
-        <v>8.8686663845379403</v>
-      </c>
+        <v>57.82</v>
+      </c>
+      <c r="G8" s="20"/>
       <c r="H8" s="1">
         <v>7</v>
       </c>
       <c r="I8" s="7">
-        <f>G8/SQRT(H8)</f>
-        <v>3.3520408163265309</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1852,7 +1714,7 @@
       <c r="F9" s="8">
         <v>113.4</v>
       </c>
-      <c r="G9" s="27"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="8"/>
       <c r="I9" s="9">
         <f>B9*2/100</f>

</xml_diff>

<commit_message>
remove (Rodrigues, 1983) and add (Cuthbertson et al., 1986) in `CBM thickness` sheet
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F45D40-CFD5-B742-943B-F1D7D8CA4586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A79C39F-3DE1-7441-8879-70FBD5382772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="9080" windowWidth="18740" windowHeight="8360" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -462,9 +462,6 @@
     <t>Van Hul et al., 2012</t>
   </si>
   <si>
-    <t>Rodrigues et al., 1983</t>
-  </si>
-  <si>
     <t>Ceafalan et al., 2019</t>
   </si>
   <si>
@@ -490,6 +487,9 @@
   </si>
   <si>
     <t>Obese N</t>
+  </si>
+  <si>
+    <t>Cuthbertson et al., 1986</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1504,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1525,7 +1525,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>3</v>
@@ -1537,7 +1537,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I1" s="23" t="s">
         <v>5</v>
@@ -1545,16 +1545,21 @@
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
+        <f>C2/SQRT(D2)</f>
+        <v>6.5</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="19"/>
       <c r="H2" s="2"/>
@@ -1562,7 +1567,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>56.78</v>
@@ -1584,7 +1589,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
         <v>73</v>
@@ -1606,7 +1611,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1">
         <v>92.87</v>
@@ -1618,7 +1623,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E8" si="0">C5/SQRT(D5)</f>
+        <f t="shared" ref="E5:E6" si="0">C5/SQRT(D5)</f>
         <v>6.6821590822128734</v>
       </c>
       <c r="F5" s="2"/>
@@ -1628,7 +1633,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1">
         <v>76.75</v>
@@ -1650,7 +1655,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
         <v>61.87</v>
@@ -1675,7 +1680,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1">
         <v>55.67</v>
@@ -1700,7 +1705,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8">
         <v>89</v>

</xml_diff>

<commit_message>
edit typo (`Calson` -> `Carlson` & `Cuthbertson et al., 1986` -> `Cuthbertson & Mandel, 1986`)
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A79C39F-3DE1-7441-8879-70FBD5382772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6F77A2-ADA1-804F-AB91-A1D5194743D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9080" windowWidth="18740" windowHeight="8360" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -468,12 +468,6 @@
     <t>Creutzfeldt et al., 1970</t>
   </si>
   <si>
-    <t>Calson et al., 2003 (muscle)</t>
-  </si>
-  <si>
-    <t>Calson et al., 2003 (retina)</t>
-  </si>
-  <si>
     <t>Lash et al., 1989 (11 wk.)</t>
   </si>
   <si>
@@ -489,7 +483,13 @@
     <t>Obese N</t>
   </si>
   <si>
-    <t>Cuthbertson et al., 1986</t>
+    <t>Carlson et al., 2003 (retina)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (muscle)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1504,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1525,7 +1525,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>3</v>
@@ -1537,7 +1537,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="23" t="s">
         <v>5</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>92.87</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1">
         <v>76.75</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
         <v>61.87</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1">
         <v>55.67</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="8">
         <v>89</v>

</xml_diff>

<commit_message>
add (Dosso, 1990) to retinal CBM thickness data
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6F77A2-ADA1-804F-AB91-A1D5194743D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD2859D-459F-704A-BD8C-8E411FE3FF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Cuthbertson &amp; Mandel, 1986</t>
+  </si>
+  <si>
+    <t>Dosso, 1990</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -749,13 +752,67 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -768,31 +825,14 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -811,7 +851,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -826,12 +865,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1191,7 +1235,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2">
@@ -1206,7 +1250,7 @@
       <c r="E2" s="6">
         <v>1.838396591281048</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1226,7 +1270,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1">
@@ -1241,7 +1285,7 @@
       <c r="E3" s="7">
         <v>5.3</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1263,7 +1307,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="1">
@@ -1276,7 +1320,7 @@
       <c r="E4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1298,7 +1342,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1">
@@ -1313,7 +1357,7 @@
       <c r="E5" s="7">
         <v>3.5</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="22" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1333,7 +1377,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="1">
@@ -1348,7 +1392,7 @@
       <c r="E6" s="7">
         <v>0.45708536881646961</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1370,7 +1414,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1">
@@ -1385,7 +1429,7 @@
       <c r="E7" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1407,7 +1451,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="1">
@@ -1424,7 +1468,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="1"/>
@@ -1437,7 +1481,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="1"/>
@@ -1453,7 +1497,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="8">
@@ -1501,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1518,33 +1562,33 @@
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="2">
@@ -1561,7 +1605,7 @@
         <v>6.5</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="19"/>
+      <c r="G2" s="18"/>
       <c r="H2" s="2"/>
       <c r="I2" s="6"/>
     </row>
@@ -1583,7 +1627,7 @@
         <v>1.25</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="19"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="1"/>
       <c r="I3" s="7"/>
     </row>
@@ -1605,7 +1649,7 @@
         <v>5.6568542494923797</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="19"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="1"/>
       <c r="I4" s="7"/>
     </row>
@@ -1627,7 +1671,7 @@
         <v>6.6821590822128734</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="19"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="1"/>
       <c r="I5" s="7"/>
     </row>
@@ -1649,7 +1693,7 @@
         <v>4.4809474444585931</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="19"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="1"/>
       <c r="I6" s="7"/>
     </row>
@@ -1670,7 +1714,7 @@
       <c r="F7" s="1">
         <v>68.13</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="1">
         <v>6</v>
       </c>
@@ -1695,7 +1739,7 @@
       <c r="F8" s="1">
         <v>57.82</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="1">
         <v>7</v>
       </c>
@@ -1703,27 +1747,58 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="24">
         <v>89</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24">
         <f>B9*2.2/100</f>
         <v>1.9580000000000002</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="24">
         <v>113.4</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9">
+      <c r="G9" s="25"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="26">
         <f>B9*2/100</f>
         <v>1.78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="28">
+        <v>93.6</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6.12</v>
+      </c>
+      <c r="D10" s="28">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <f>C10/SQRT(D10)</f>
+        <v>2.7369472044597427</v>
+      </c>
+      <c r="F10" s="28">
+        <v>104.6</v>
+      </c>
+      <c r="G10" s="28">
+        <v>4.58</v>
+      </c>
+      <c r="H10" s="8">
+        <v>4</v>
+      </c>
+      <c r="I10" s="9">
+        <f>G10/SQRT(H10)</f>
+        <v>2.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete (Danis & Yang, 1993) data from CBM thickness of obese rat because the rats are diabetic
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD2859D-459F-704A-BD8C-8E411FE3FF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B60D26-B55C-0C4C-9656-AFAE4CB95918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -832,7 +832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -867,15 +867,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1250,7 +1249,7 @@
       <c r="E2" s="6">
         <v>1.838396591281048</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="27" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1285,7 +1284,7 @@
       <c r="E3" s="7">
         <v>5.3</v>
       </c>
-      <c r="G3" s="22"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1320,7 +1319,7 @@
       <c r="E4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1357,7 +1356,7 @@
       <c r="E5" s="7">
         <v>3.5</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="27" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1392,7 +1391,7 @@
       <c r="E6" s="7">
         <v>0.45708536881646961</v>
       </c>
-      <c r="G6" s="22"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1429,7 +1428,7 @@
       <c r="E7" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G7" s="22"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1548,7 +1547,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F9" sqref="F9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1748,49 +1747,44 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>89</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23">
         <f>B9*2.2/100</f>
         <v>1.9580000000000002</v>
       </c>
-      <c r="F9" s="24">
-        <v>113.4</v>
-      </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="26">
-        <f>B9*2/100</f>
-        <v>1.78</v>
-      </c>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="8">
         <v>93.6</v>
       </c>
       <c r="C10" s="8">
         <v>6.12</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="8">
         <v>5</v>
       </c>
       <c r="E10" s="8">
         <f>C10/SQRT(D10)</f>
         <v>2.7369472044597427</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="8">
         <v>104.6</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="8">
         <v>4.58</v>
       </c>
       <c r="H10" s="8">

</xml_diff>

<commit_message>
edit the name of reference `Dosso, 1990` -> `Dosso et al., 1990`
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B60D26-B55C-0C4C-9656-AFAE4CB95918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F388EA5-DEBB-0D40-95E4-0F54EBAD29C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -492,7 +492,7 @@
     <t>Cuthbertson &amp; Mandel, 1986</t>
   </si>
   <si>
-    <t>Dosso, 1990</t>
+    <t>Dosso et al., 1990</t>
   </si>
 </sst>
 </file>
@@ -1547,7 +1547,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:I9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add more CBM thickness data
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F388EA5-DEBB-0D40-95E4-0F54EBAD29C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26C9FE5-5307-9746-91B9-E26686863E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="14700" windowHeight="16680" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{C4AAA6B2-9BD9-1746-AF06-F09AA047F1D1}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{C4AAA6B2-9BD9-1746-AF06-F09AA047F1D1}">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{57820837-87CC-154D-ABDA-2F7B7F8DAB0C}">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{57820837-87CC-154D-ABDA-2F7B7F8DAB0C}">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{268D93CA-546C-014C-BD5E-79D88978D419}">
+    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{268D93CA-546C-014C-BD5E-79D88978D419}">
       <text>
         <r>
           <rPr>
@@ -204,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{BECC8C1A-53BD-B344-8091-D3346FF7CCDC}">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{BECC8C1A-53BD-B344-8091-D3346FF7CCDC}">
       <text>
         <r>
           <rPr>
@@ -237,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{C5458797-ECBF-C24D-B558-39DD5A3F08D9}">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{C5458797-ECBF-C24D-B558-39DD5A3F08D9}">
       <text>
         <r>
           <rPr>
@@ -270,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{5B8BC328-C175-1645-944D-85396FC5B1C5}">
+    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{5B8BC328-C175-1645-944D-85396FC5B1C5}">
       <text>
         <r>
           <rPr>
@@ -333,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
+    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
       <text>
         <r>
           <rPr>
@@ -391,7 +391,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -462,44 +462,161 @@
     <t>Van Hul et al., 2012</t>
   </si>
   <si>
-    <t>Ceafalan et al., 2019</t>
-  </si>
-  <si>
-    <t>Creutzfeldt et al., 1970</t>
-  </si>
-  <si>
-    <t>Lash et al., 1989 (11 wk.)</t>
-  </si>
-  <si>
-    <t>Lash et al., 1989 (18 wk.)</t>
-  </si>
-  <si>
-    <t>Danis &amp; Yang, 1993</t>
-  </si>
-  <si>
     <t>Lean N</t>
   </si>
   <si>
     <t>Obese N</t>
   </si>
   <si>
-    <t>Carlson et al., 2003 (retina)</t>
-  </si>
-  <si>
-    <t>Carlson et al., 2003 (muscle)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986</t>
-  </si>
-  <si>
-    <t>Dosso et al., 1990</t>
+    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, periphery zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, center zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. CBA mice &amp; Retina, mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (4 mo. CBA mice &amp; Retina, mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (8 mo. CBA mice &amp; Retina, mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (12 mo. CBA mice &amp; Retina, mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (20 mo. CBA mice &amp; Retina, mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (8 mo. Balb/c mice &amp; Retina, mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (20 mo. Balb/c mice &amp; Retina, mid-zone)</t>
+  </si>
+  <si>
+    <t>Rodrigues et al., 1983 (7 mo. SJL/J mice &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Creutzfeldt et al., 1970 (7 mo. Spiny mice &amp; Muscle)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Muscle)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Pulmonary alveolus)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Diphragm)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Pancreas)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Choroid)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Heart IVS)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Heart LV)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Peripheral nerve)</t>
+  </si>
+  <si>
+    <t>Williams et al., 2020 (5.5 mo. C57Bl/6 mice &amp; Muscle)</t>
+  </si>
+  <si>
+    <t>Chang et al., 2012 (7.5 mo. FVB/NJ mice &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Velic et al., 2013 (12 mo. FVB mice &amp; Heart LV)</t>
+  </si>
+  <si>
+    <t>Lash et al., 1989 (2.8 mo. Zucker rat &amp; Muscle)</t>
+  </si>
+  <si>
+    <t>Lash et al., 1989 (4.5 mo. Zucker rat &amp; Muscle)</t>
+  </si>
+  <si>
+    <t>Cherian et al., 2009 (6 mo. Sprague-Dawley rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Danis &amp; Yang, 1993 (6.5 mo. Zucker rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Gambaro et al., 1992 (9.5 mo. Sprague-Dawley rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (1 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (2 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (3 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (4 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (5 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (6 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (7 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (8 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Yagihashi, 1978 (9 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Fox et al., 1977 (17 mo. Wistar rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Saito et al., 2003 (5.5 mo. LEFT rat &amp; Heart)</t>
+  </si>
+  <si>
+    <t>Begieneman et al., 2009 (Rat &amp; Heart LV)</t>
+  </si>
+  <si>
+    <t>Saito et al., 2003 (15.5 mo. LEFT rat &amp; Heart)</t>
+  </si>
+  <si>
+    <t>Ceafalan et al., 2019 (6 mo. C57Bl/6J mice &amp; Brain)</t>
+  </si>
+  <si>
+    <t>Ceafalan et al., 2019 (24 mo. C57Bl/6J mice &amp; Brain)</t>
+  </si>
+  <si>
+    <t>Dosso et al., 1990 (17 mo. Zucker rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Fraselle-Jacobs et al., 1987 (6 mo. Wistar rat &amp; Adipose)</t>
+  </si>
+  <si>
+    <t>Cherian et al., 2009 (6 mo. Sprague-Dawley rat &amp; Kidney)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -520,6 +637,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -529,7 +653,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -739,49 +863,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -798,10 +879,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -809,30 +892,19 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -865,16 +937,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1249,7 +1322,7 @@
       <c r="E2" s="6">
         <v>1.838396591281048</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="20" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1284,7 +1357,7 @@
       <c r="E3" s="7">
         <v>5.3</v>
       </c>
-      <c r="G3" s="27"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1319,7 +1392,7 @@
       <c r="E4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1356,7 +1429,7 @@
       <c r="E5" s="7">
         <v>3.5</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="20" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1391,7 +1464,7 @@
       <c r="E6" s="7">
         <v>0.45708536881646961</v>
       </c>
-      <c r="G6" s="27"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1428,7 +1501,7 @@
       <c r="E7" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1544,15 +1617,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1568,7 +1641,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>3</v>
@@ -1579,29 +1652,29 @@
       <c r="G1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="21" t="s">
+      <c r="H1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="2">
-        <v>59</v>
-      </c>
-      <c r="C2" s="2">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2">
+        <v>27</v>
+      </c>
+      <c r="B2" s="22">
+        <v>50</v>
+      </c>
+      <c r="C2" s="22">
+        <v>9</v>
+      </c>
+      <c r="D2" s="23">
         <v>4</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="23">
         <f>C2/SQRT(D2)</f>
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="18"/>
@@ -1609,191 +1682,1055 @@
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1">
-        <v>56.78</v>
-      </c>
-      <c r="C3" s="1">
-        <v>12.5</v>
+      <c r="A3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2">
+        <v>59</v>
+      </c>
+      <c r="C3" s="2">
+        <v>13</v>
       </c>
       <c r="D3" s="2">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2">
-        <f>C3/SQRT(D3)</f>
-        <v>1.25</v>
+        <f t="shared" ref="E3:E25" si="0">C3/SQRT(D3)</f>
+        <v>6.5</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="7"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1">
-        <v>73</v>
-      </c>
-      <c r="C4" s="1">
-        <v>16</v>
+      <c r="A4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2">
+        <v>75</v>
+      </c>
+      <c r="C4" s="2">
+        <v>10</v>
       </c>
       <c r="D4" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2">
-        <f>C4/SQRT(D4)</f>
-        <v>5.6568542494923797</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="7"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1">
-        <v>92.87</v>
-      </c>
-      <c r="C5" s="1">
-        <v>18.899999999999999</v>
+      <c r="B5" s="2">
+        <v>108</v>
+      </c>
+      <c r="C5" s="2">
+        <v>17</v>
       </c>
       <c r="D5" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E6" si="0">C5/SQRT(D5)</f>
-        <v>6.6821590822128734</v>
+        <f t="shared" si="0"/>
+        <v>8.5</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="18"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1">
-        <v>76.75</v>
-      </c>
-      <c r="C6" s="1">
-        <v>14.17</v>
+      <c r="B6" s="2">
+        <v>154</v>
+      </c>
+      <c r="C6" s="2">
+        <v>27</v>
       </c>
       <c r="D6" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>4.4809474444585931</v>
+        <v>13.5</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2">
+        <v>55</v>
+      </c>
+      <c r="C7" s="2">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>6.3639610306789276</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2">
+        <v>77</v>
+      </c>
+      <c r="C8" s="2">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>6.3639610306789276</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2">
+        <v>158</v>
+      </c>
+      <c r="C9" s="2">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>24.748737341529161</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B11" s="2">
+        <v>64</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2">
+        <v>91</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>12</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.86602540378443871</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="1">
+        <v>56.78</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>100</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="1">
+        <v>107.53</v>
+      </c>
+      <c r="C14" s="1">
+        <v>23.76</v>
+      </c>
+      <c r="D14" s="2">
+        <v>100</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>2.3760000000000003</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1">
+        <v>73</v>
+      </c>
+      <c r="C15" s="1">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>5.6568542494923797</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1">
+        <v>92.87</v>
+      </c>
+      <c r="C16" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>6.6821590822128734</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1">
+        <v>76.75</v>
+      </c>
+      <c r="C17" s="1">
+        <v>14.17</v>
+      </c>
+      <c r="D17" s="2">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4809474444585931</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1">
+        <v>178.16</v>
+      </c>
+      <c r="C18" s="1">
+        <v>35.61</v>
+      </c>
+      <c r="D18" s="2">
+        <v>19</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>8.1694942831307031</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1">
+        <v>67.989999999999995</v>
+      </c>
+      <c r="C19" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="D19" s="2">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>2.4571960646232527</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1">
+        <v>54.75</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7677669529663687</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1">
+        <v>103.54</v>
+      </c>
+      <c r="C21" s="1">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="D21" s="2">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>5.77352686838816</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1">
+        <v>78.58</v>
+      </c>
+      <c r="C22" s="1">
+        <v>7.06</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0760929004787583</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1">
+        <v>63.13</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5.91</v>
+      </c>
+      <c r="D23" s="2">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7060700454553444</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1">
+        <v>56.92</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="D24" s="2">
+        <v>12</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1604740410711478</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1">
+        <v>58.75</v>
+      </c>
+      <c r="C25" s="1">
+        <v>9.86</v>
+      </c>
+      <c r="D25" s="2">
+        <v>15</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>2.5458410529070084</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1">
+        <v>107.62</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1">
+        <v>31</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5.4820000000000002</v>
+      </c>
+      <c r="F26" s="1">
+        <v>102.7</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <v>31</v>
+      </c>
+      <c r="I26" s="7">
+        <v>6.44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1">
+        <v>224.2</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+      <c r="E27" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1">
+        <v>48.5</v>
+      </c>
+      <c r="C28" s="1">
+        <v>7.31</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1">
+        <f>C28/SQRT(D28)</f>
+        <v>2.762920297697451</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1">
         <v>61.87</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1">
         <v>6</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E29" s="1">
         <v>1.33</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F29" s="1">
         <v>68.13</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="1">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1">
         <v>6</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I29" s="7">
         <v>1.66</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1">
         <v>55.67</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1">
         <v>6</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E30" s="1">
         <v>1.04</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F30" s="1">
         <v>57.82</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="1">
+      <c r="G30" s="1"/>
+      <c r="H30" s="1">
         <v>7</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I30" s="7">
         <v>1.24</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="23">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="1">
+        <v>93.6</v>
+      </c>
+      <c r="C31" s="1">
+        <v>6.12</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1">
+        <f>C31/SQRT(D31)</f>
+        <v>2.7369472044597427</v>
+      </c>
+      <c r="F31" s="1">
+        <v>104.6</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4.58</v>
+      </c>
+      <c r="H31" s="1">
+        <v>4</v>
+      </c>
+      <c r="I31" s="7">
+        <f>G31/SQRT(H31)</f>
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="1">
+        <v>108.78</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="1">
         <v>89</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23">
-        <f>B9*2.2/100</f>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1">
+        <f>B33*2.2/100</f>
         <v>1.9580000000000002</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="25"/>
-    </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="8">
-        <v>93.6</v>
-      </c>
-      <c r="C10" s="8">
-        <v>6.12</v>
-      </c>
-      <c r="D10" s="8">
-        <v>5</v>
-      </c>
-      <c r="E10" s="8">
-        <f>C10/SQRT(D10)</f>
-        <v>2.7369472044597427</v>
-      </c>
-      <c r="F10" s="8">
-        <v>104.6</v>
-      </c>
-      <c r="G10" s="8">
-        <v>4.58</v>
-      </c>
-      <c r="H10" s="8">
+      <c r="F33" s="1">
+        <v>113.4</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="7">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="1">
+        <v>50.8</v>
+      </c>
+      <c r="C34" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6</v>
+      </c>
+      <c r="E34" s="1">
+        <f>C34/SQRT(D34)</f>
+        <v>2.0820662813657016</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="1">
+        <v>81</v>
+      </c>
+      <c r="C35" s="1">
+        <v>9.9</v>
+      </c>
+      <c r="D35" s="1">
+        <v>6</v>
+      </c>
+      <c r="E35" s="1">
+        <f>C35/SQRT(D35)</f>
+        <v>4.0416580755922444</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="25">
+        <v>235.57</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="1">
+        <v>119</v>
+      </c>
+      <c r="C37" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="D37" s="1">
         <v>4</v>
       </c>
-      <c r="I10" s="9">
-        <f>G10/SQRT(H10)</f>
-        <v>2.29</v>
-      </c>
+      <c r="E37" s="1">
+        <f>C37/SQRT(D37)</f>
+        <v>3.4</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="1">
+        <v>129.1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D38" s="1">
+        <v>4</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" ref="E38:E48" si="1">C38/SQRT(D38)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="1">
+        <v>135.4</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D39" s="1">
+        <v>4</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="1">
+        <v>147.30000000000001</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="1">
+        <v>154.1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D41" s="1">
+        <v>4</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="1">
+        <v>160.5</v>
+      </c>
+      <c r="C42" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="D42" s="1">
+        <v>4</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="1">
+        <v>184.6</v>
+      </c>
+      <c r="C43" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="D43" s="1">
+        <v>4</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="1"/>
+        <v>3.25</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="1">
+        <v>205.3</v>
+      </c>
+      <c r="C44" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="D44" s="1">
+        <v>4</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="1">
+        <v>238.3</v>
+      </c>
+      <c r="C45" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="D45" s="1">
+        <v>4</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="1">
+        <v>305</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1">
+        <v>6</v>
+      </c>
+      <c r="E46" s="1">
+        <v>10</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="1">
+        <v>90</v>
+      </c>
+      <c r="C47" s="1">
+        <v>12</v>
+      </c>
+      <c r="D47" s="1">
+        <v>50</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="1"/>
+        <v>1.697056274847714</v>
+      </c>
+      <c r="F47" s="1">
+        <v>106</v>
+      </c>
+      <c r="G47" s="1">
+        <v>20</v>
+      </c>
+      <c r="H47" s="1">
+        <v>50</v>
+      </c>
+      <c r="I47" s="7">
+        <f>G47/SQRT(H47)</f>
+        <v>2.8284271247461898</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="19">
+        <v>87</v>
+      </c>
+      <c r="C48" s="19">
+        <v>12</v>
+      </c>
+      <c r="D48" s="19">
+        <v>50</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="1"/>
+        <v>1.697056274847714</v>
+      </c>
+      <c r="F48" s="19">
+        <v>177</v>
+      </c>
+      <c r="G48" s="19">
+        <v>66</v>
+      </c>
+      <c r="H48" s="19">
+        <v>50</v>
+      </c>
+      <c r="I48" s="7">
+        <f>G48/SQRT(H48)</f>
+        <v>9.3338095116624267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="8">
+        <v>68.736000000000004</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8">
+        <v>6</v>
+      </c>
+      <c r="E49" s="8">
+        <v>4.22</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edit reference names (`Heart LV` -> `Heart` except Carlson et al., 2003) for Carlson et al., 2003 `Heart **` -> `Heart, **`
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26C9FE5-5307-9746-91B9-E26686863E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D7F2E3-0BF5-7C41-A3DF-813D3552CD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="14700" windowHeight="16680" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -525,12 +525,6 @@
     <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Choroid)</t>
   </si>
   <si>
-    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Heart IVS)</t>
-  </si>
-  <si>
-    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Heart LV)</t>
-  </si>
-  <si>
     <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Peripheral nerve)</t>
   </si>
   <si>
@@ -540,9 +534,6 @@
     <t>Chang et al., 2012 (7.5 mo. FVB/NJ mice &amp; Kidney)</t>
   </si>
   <si>
-    <t>Velic et al., 2013 (12 mo. FVB mice &amp; Heart LV)</t>
-  </si>
-  <si>
     <t>Lash et al., 1989 (2.8 mo. Zucker rat &amp; Muscle)</t>
   </si>
   <si>
@@ -591,7 +582,7 @@
     <t>Saito et al., 2003 (5.5 mo. LEFT rat &amp; Heart)</t>
   </si>
   <si>
-    <t>Begieneman et al., 2009 (Rat &amp; Heart LV)</t>
+    <t>Begieneman et al., 2009 (Rat &amp; Heart)</t>
   </si>
   <si>
     <t>Saito et al., 2003 (15.5 mo. LEFT rat &amp; Heart)</t>
@@ -610,6 +601,15 @@
   </si>
   <si>
     <t>Cherian et al., 2009 (6 mo. Sprague-Dawley rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Heart, IVS)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Heart, LV)</t>
+  </si>
+  <si>
+    <t>Velic et al., 2013 (12 mo. FVB mice &amp; Heart)</t>
   </si>
 </sst>
 </file>
@@ -1619,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1">
         <v>56.78</v>
@@ -1925,7 +1925,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1">
         <v>107.53</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="B23" s="1">
         <v>63.13</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1">
         <v>56.92</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1">
         <v>58.75</v>
@@ -2189,7 +2189,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="1">
         <v>107.62</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B27" s="1">
         <v>224.2</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B28" s="1">
         <v>48.5</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1">
         <v>61.87</v>
@@ -2280,7 +2280,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B30" s="1">
         <v>55.67</v>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" s="1">
         <v>93.6</v>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B32" s="1">
         <v>108.78</v>
@@ -2353,7 +2353,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1">
         <v>89</v>
@@ -2375,7 +2375,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B34" s="1">
         <v>50.8</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1">
         <v>81</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B36" s="25">
         <v>235.57</v>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B37" s="1">
         <v>119</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B38" s="1">
         <v>129.1</v>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B39" s="1">
         <v>135.4</v>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B40" s="1">
         <v>147.30000000000001</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B41" s="1">
         <v>154.1</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B42" s="1">
         <v>160.5</v>
@@ -2568,7 +2568,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B43" s="1">
         <v>184.6</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B44" s="1">
         <v>205.3</v>
@@ -2612,7 +2612,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B45" s="1">
         <v>238.3</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B46" s="1">
         <v>305</v>
@@ -2653,7 +2653,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B47" s="1">
         <v>90</v>
@@ -2684,7 +2684,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B48" s="19">
         <v>87</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="49" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B49" s="8">
         <v>68.736000000000004</v>

</xml_diff>

<commit_message>
edit reference name in Carlson et al., 2003: 1. Fix typo (`Diphgram` -> `Di"a"phgram`) 2. Add `Extensor digitorum` to `Carlson et al., 2003 ... (Muscle)` 3. Add `Muscle` to `Carlson et al., 2003 ... (Diaphgram)`
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D7F2E3-0BF5-7C41-A3DF-813D3552CD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9DF009-4FA6-E84C-B147-7DF2EA983AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -507,18 +507,12 @@
     <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Retina)</t>
   </si>
   <si>
-    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Muscle)</t>
-  </si>
-  <si>
     <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Kidney)</t>
   </si>
   <si>
     <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Pulmonary alveolus)</t>
   </si>
   <si>
-    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Diphragm)</t>
-  </si>
-  <si>
     <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Pancreas)</t>
   </si>
   <si>
@@ -610,6 +604,12 @@
   </si>
   <si>
     <t>Velic et al., 2013 (12 mo. FVB mice &amp; Heart)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Muscle, Extensor digitorum)</t>
+  </si>
+  <si>
+    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Muscle, Diaphragm)</t>
   </si>
 </sst>
 </file>
@@ -904,7 +904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -937,17 +937,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1322,7 +1320,7 @@
       <c r="E2" s="6">
         <v>1.838396591281048</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1357,7 +1355,7 @@
       <c r="E3" s="7">
         <v>5.3</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1392,7 +1390,7 @@
       <c r="E4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1429,7 +1427,7 @@
       <c r="E5" s="7">
         <v>3.5</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="26" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1464,7 +1462,7 @@
       <c r="E6" s="7">
         <v>0.45708536881646961</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1501,7 +1499,7 @@
       <c r="E7" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1619,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1655,7 +1653,7 @@
       <c r="H1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1663,16 +1661,16 @@
       <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="21">
         <v>50</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="21">
         <v>9</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="22">
         <v>4</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="22">
         <f>C2/SQRT(D2)</f>
         <v>4.5</v>
       </c>
@@ -1726,7 +1724,7 @@
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="2">
@@ -1748,7 +1746,7 @@
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="2">
@@ -1770,7 +1768,7 @@
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="2">
@@ -1792,7 +1790,7 @@
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="2">
@@ -1814,7 +1812,7 @@
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="2">
@@ -1836,7 +1834,7 @@
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="2">
@@ -1858,7 +1856,7 @@
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="2">
@@ -1903,7 +1901,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1">
         <v>56.78</v>
@@ -1925,7 +1923,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1">
         <v>107.53</v>
@@ -1991,7 +1989,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1">
         <v>76.75</v>
@@ -2012,8 +2010,8 @@
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
-        <v>39</v>
+      <c r="A18" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="B18" s="1">
         <v>178.16</v>
@@ -2034,8 +2032,8 @@
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="24" t="s">
-        <v>40</v>
+      <c r="A19" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="B19" s="1">
         <v>67.989999999999995</v>
@@ -2056,8 +2054,8 @@
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
-        <v>41</v>
+      <c r="A20" s="23" t="s">
+        <v>72</v>
       </c>
       <c r="B20" s="1">
         <v>54.75</v>
@@ -2078,8 +2076,8 @@
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
-        <v>42</v>
+      <c r="A21" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="B21" s="1">
         <v>103.54</v>
@@ -2100,8 +2098,8 @@
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
-        <v>43</v>
+      <c r="A22" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="B22" s="1">
         <v>78.58</v>
@@ -2122,8 +2120,8 @@
       <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
-        <v>70</v>
+      <c r="A23" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="B23" s="1">
         <v>63.13</v>
@@ -2144,8 +2142,8 @@
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
-        <v>71</v>
+      <c r="A24" s="23" t="s">
+        <v>69</v>
       </c>
       <c r="B24" s="1">
         <v>56.92</v>
@@ -2167,7 +2165,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1">
         <v>58.75</v>
@@ -2189,7 +2187,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1">
         <v>107.62</v>
@@ -2214,7 +2212,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1">
         <v>224.2</v>
@@ -2233,7 +2231,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B28" s="1">
         <v>48.5</v>
@@ -2255,7 +2253,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1">
         <v>61.87</v>
@@ -2280,7 +2278,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1">
         <v>55.67</v>
@@ -2305,7 +2303,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B31" s="1">
         <v>93.6</v>
@@ -2336,7 +2334,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1">
         <v>108.78</v>
@@ -2353,7 +2351,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B33" s="1">
         <v>89</v>
@@ -2375,7 +2373,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1">
         <v>50.8</v>
@@ -2397,7 +2395,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1">
         <v>81</v>
@@ -2418,10 +2416,10 @@
       <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="25">
+      <c r="A36" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="1">
         <v>235.57</v>
       </c>
       <c r="C36" s="1"/>
@@ -2436,7 +2434,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B37" s="1">
         <v>119</v>
@@ -2458,7 +2456,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B38" s="1">
         <v>129.1</v>
@@ -2480,7 +2478,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B39" s="1">
         <v>135.4</v>
@@ -2502,7 +2500,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B40" s="1">
         <v>147.30000000000001</v>
@@ -2524,7 +2522,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B41" s="1">
         <v>154.1</v>
@@ -2546,7 +2544,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B42" s="1">
         <v>160.5</v>
@@ -2568,7 +2566,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B43" s="1">
         <v>184.6</v>
@@ -2589,8 +2587,8 @@
       <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="24" t="s">
-        <v>59</v>
+      <c r="A44" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="B44" s="1">
         <v>205.3</v>
@@ -2611,8 +2609,8 @@
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="24" t="s">
-        <v>60</v>
+      <c r="A45" s="23" t="s">
+        <v>58</v>
       </c>
       <c r="B45" s="1">
         <v>238.3</v>
@@ -2633,8 +2631,8 @@
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="27" t="s">
-        <v>61</v>
+      <c r="A46" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="B46" s="1">
         <v>305</v>
@@ -2652,8 +2650,8 @@
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="27" t="s">
-        <v>62</v>
+      <c r="A47" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="B47" s="1">
         <v>90</v>
@@ -2683,8 +2681,8 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="27" t="s">
-        <v>64</v>
+      <c r="A48" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="B48" s="19">
         <v>87</v>
@@ -2714,8 +2712,8 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>63</v>
+      <c r="A49" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="B49" s="8">
         <v>68.736000000000004</v>

</xml_diff>

<commit_message>
use capital letter for `Mid-`, `Center` and `Peripheral` in Cuthbertson's paper
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9DF009-4FA6-E84C-B147-7DF2EA983AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543E548D-FC93-E840-A99D-40FD96D65760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -468,36 +468,6 @@
     <t>Obese N</t>
   </si>
   <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, periphery zone)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, center zone)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. CBA mice &amp; Retina, mid-zone)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (4 mo. CBA mice &amp; Retina, mid-zone)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (8 mo. CBA mice &amp; Retina, mid-zone)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (12 mo. CBA mice &amp; Retina, mid-zone)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (20 mo. CBA mice &amp; Retina, mid-zone)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, mid-zone)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (8 mo. Balb/c mice &amp; Retina, mid-zone)</t>
-  </si>
-  <si>
-    <t>Cuthbertson &amp; Mandel, 1986 (20 mo. Balb/c mice &amp; Retina, mid-zone)</t>
-  </si>
-  <si>
     <t>Rodrigues et al., 1983 (7 mo. SJL/J mice &amp; Kidney)</t>
   </si>
   <si>
@@ -610,6 +580,36 @@
   </si>
   <si>
     <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Muscle, Diaphragm)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. CBA mice &amp; Retina, Mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (4 mo. CBA mice &amp; Retina, Mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (8 mo. CBA mice &amp; Retina, Mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (12 mo. CBA mice &amp; Retina, Mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (20 mo. CBA mice &amp; Retina, Mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (8 mo. Balb/c mice &amp; Retina, Mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (20 mo. Balb/c mice &amp; Retina, Mid-zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, Center zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, Periphery zone)</t>
+  </si>
+  <si>
+    <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, Mid-zone)</t>
   </si>
 </sst>
 </file>
@@ -1617,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="B2" s="21">
         <v>50</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2">
         <v>59</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2">
         <v>75</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2">
         <v>108</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="B6" s="2">
         <v>154</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2">
         <v>55</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="B8" s="2">
         <v>77</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="B9" s="2">
         <v>158</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="B10" s="2">
         <v>41</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="B11" s="2">
         <v>64</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2">
         <v>91</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1">
         <v>56.78</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1">
         <v>107.53</v>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>73</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1">
         <v>92.87</v>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1">
         <v>76.75</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1">
         <v>178.16</v>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1">
         <v>67.989999999999995</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1">
         <v>54.75</v>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1">
         <v>103.54</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>78.58</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1">
         <v>63.13</v>
@@ -2143,7 +2143,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B24" s="1">
         <v>56.92</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1">
         <v>58.75</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1">
         <v>107.62</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1">
         <v>224.2</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1">
         <v>48.5</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1">
         <v>61.87</v>
@@ -2278,7 +2278,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1">
         <v>55.67</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1">
         <v>93.6</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B32" s="1">
         <v>108.78</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1">
         <v>89</v>
@@ -2368,12 +2368,13 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="7">
+        <f>B33*2/100</f>
         <v>1.78</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1">
         <v>50.8</v>
@@ -2395,7 +2396,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1">
         <v>81</v>
@@ -2417,7 +2418,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1">
         <v>235.57</v>
@@ -2434,7 +2435,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1">
         <v>119</v>
@@ -2456,7 +2457,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1">
         <v>129.1</v>
@@ -2478,7 +2479,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1">
         <v>135.4</v>
@@ -2500,7 +2501,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1">
         <v>147.30000000000001</v>
@@ -2522,7 +2523,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1">
         <v>154.1</v>
@@ -2544,7 +2545,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B42" s="1">
         <v>160.5</v>
@@ -2566,7 +2567,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B43" s="1">
         <v>184.6</v>
@@ -2588,7 +2589,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1">
         <v>205.3</v>
@@ -2610,7 +2611,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B45" s="1">
         <v>238.3</v>
@@ -2632,7 +2633,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B46" s="1">
         <v>305</v>
@@ -2651,7 +2652,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1">
         <v>90</v>
@@ -2682,7 +2683,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B48" s="19">
         <v>87</v>
@@ -2713,7 +2714,7 @@
     </row>
     <row r="49" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B49" s="8">
         <v>68.736000000000004</v>

</xml_diff>

<commit_message>
add missing data in `Lijnen et al., 2001` and `Voros et al., 2005`
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543E548D-FC93-E840-A99D-40FD96D65760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1784E6B0-AE73-614E-9F0C-75AF233E7F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -435,18 +435,12 @@
     <t>Lijnen et al., 2006</t>
   </si>
   <si>
-    <t>Lijnen et al., 2001</t>
-  </si>
-  <si>
     <t>Maquoi et al., 2002</t>
   </si>
   <si>
     <t>Morange et al.,2000</t>
   </si>
   <si>
-    <t>Voros et al., 2005</t>
-  </si>
-  <si>
     <t>Lijnen, Maquoi et al., 2003</t>
   </si>
   <si>
@@ -610,6 +604,21 @@
   </si>
   <si>
     <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, Mid-zone)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (15 wk. mice)</t>
+  </si>
+  <si>
+    <t>Lijnen et al., 2001 (22 wk. mice)</t>
+  </si>
+  <si>
+    <t>Lijnen et al., 2001 (37 wk. mice)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (7 wk. mice)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (10 wk. mice)</t>
   </si>
 </sst>
 </file>
@@ -1260,15 +1269,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C9A479-2AA3-884B-8FF7-FA729F57839B}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1341,7 +1350,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1">
         <v>49</v>
@@ -1378,17 +1387,15 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E4" s="7">
-        <v>3</v>
+        <v>1.6</v>
       </c>
       <c r="G4" s="26"/>
       <c r="H4" s="1" t="s">
@@ -1413,19 +1420,17 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>49</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4.3</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E5" s="7">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>1</v>
@@ -1448,19 +1453,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
-        <v>28.76813695875796</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0622081338618323</v>
+        <v>4.3</v>
       </c>
       <c r="D6" s="1">
-        <v>52.925674284012274</v>
+        <v>82</v>
       </c>
       <c r="E6" s="7">
-        <v>0.45708536881646961</v>
+        <v>3.5</v>
       </c>
       <c r="G6" s="26"/>
       <c r="H6" s="1" t="s">
@@ -1485,19 +1490,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B7" s="1">
-        <v>62</v>
+        <v>21.41</v>
       </c>
       <c r="C7" s="1">
-        <v>4.0999999999999996</v>
+        <v>0.83</v>
       </c>
       <c r="D7" s="1">
-        <v>85</v>
+        <v>34.6</v>
       </c>
       <c r="E7" s="7">
-        <v>2.2999999999999998</v>
+        <v>0.72</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="1" t="s">
@@ -1522,68 +1527,87 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1">
-        <v>40.049999999999997</v>
+        <v>26.94</v>
       </c>
       <c r="C8" s="1">
-        <v>0.76</v>
+        <v>0.47</v>
       </c>
       <c r="D8" s="1">
-        <v>94.61</v>
+        <v>40.68</v>
       </c>
       <c r="E8" s="7">
-        <v>4.58</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="B9" s="1">
+        <v>28.76813695875796</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.0622081338618323</v>
+      </c>
       <c r="D9" s="1">
-        <v>76.36</v>
+        <v>52.925674284012274</v>
       </c>
       <c r="E9" s="7">
-        <v>2.25</v>
+        <v>0.45708536881646961</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>62</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4.0999999999999996</v>
+      </c>
       <c r="D10" s="1">
-        <v>89.13</v>
+        <v>85</v>
       </c>
       <c r="E10" s="7">
-        <v>1.46</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="8">
-        <v>42.4</v>
-      </c>
-      <c r="C11" s="8">
-        <v>1.95</v>
-      </c>
-      <c r="D11" s="8">
-        <v>58.37</v>
-      </c>
-      <c r="E11" s="9">
-        <v>2.2200000000000002</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1">
+        <v>40.049999999999997</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="D11" s="1">
+        <v>94.61</v>
+      </c>
+      <c r="E11" s="7">
+        <v>4.58</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <v>76.36</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2.25</v>
+      </c>
       <c r="I12">
         <f>SQRT((I5+J5)/PI())*2</f>
         <v>29.811427376513585</v>
@@ -1594,6 +1618,17 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1">
+        <v>89.13</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.46</v>
+      </c>
       <c r="I13">
         <f>SQRT((I5-J5)/PI())*2</f>
         <v>27.685559519911603</v>
@@ -1601,6 +1636,23 @@
       <c r="K13">
         <f>SQRT((K5-L5)/PI())*2</f>
         <v>52.46659790492825</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8">
+        <v>42.4</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1.95</v>
+      </c>
+      <c r="D14" s="8">
+        <v>58.37</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2.2200000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1617,7 +1669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1639,7 +1691,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>3</v>
@@ -1651,7 +1703,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>5</v>
@@ -1659,7 +1711,7 @@
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="21">
         <v>50</v>
@@ -1681,7 +1733,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2">
         <v>59</v>
@@ -1703,7 +1755,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2">
         <v>75</v>
@@ -1725,7 +1777,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2">
         <v>108</v>
@@ -1747,7 +1799,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2">
         <v>154</v>
@@ -1769,7 +1821,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2">
         <v>55</v>
@@ -1791,7 +1843,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2">
         <v>77</v>
@@ -1813,7 +1865,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="2">
         <v>158</v>
@@ -1835,7 +1887,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B10" s="2">
         <v>41</v>
@@ -1857,7 +1909,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="2">
         <v>64</v>
@@ -1879,7 +1931,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2">
         <v>91</v>
@@ -1901,7 +1953,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1">
         <v>56.78</v>
@@ -1923,7 +1975,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1">
         <v>107.53</v>
@@ -1945,7 +1997,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1">
         <v>73</v>
@@ -1967,7 +2019,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1">
         <v>92.87</v>
@@ -1989,7 +2041,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1">
         <v>76.75</v>
@@ -2011,7 +2063,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1">
         <v>178.16</v>
@@ -2033,7 +2085,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1">
         <v>67.989999999999995</v>
@@ -2055,7 +2107,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1">
         <v>54.75</v>
@@ -2077,7 +2129,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1">
         <v>103.54</v>
@@ -2099,7 +2151,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1">
         <v>78.58</v>
@@ -2121,7 +2173,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1">
         <v>63.13</v>
@@ -2143,7 +2195,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1">
         <v>56.92</v>
@@ -2165,7 +2217,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1">
         <v>58.75</v>
@@ -2187,7 +2239,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1">
         <v>107.62</v>
@@ -2212,7 +2264,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1">
         <v>224.2</v>
@@ -2231,7 +2283,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1">
         <v>48.5</v>
@@ -2253,7 +2305,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1">
         <v>61.87</v>
@@ -2278,7 +2330,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1">
         <v>55.67</v>
@@ -2303,7 +2355,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B31" s="1">
         <v>93.6</v>
@@ -2334,7 +2386,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B32" s="1">
         <v>108.78</v>
@@ -2351,7 +2403,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1">
         <v>89</v>
@@ -2374,7 +2426,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1">
         <v>50.8</v>
@@ -2396,7 +2448,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B35" s="1">
         <v>81</v>
@@ -2418,7 +2470,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1">
         <v>235.57</v>
@@ -2435,7 +2487,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1">
         <v>119</v>
@@ -2457,7 +2509,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1">
         <v>129.1</v>
@@ -2479,7 +2531,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1">
         <v>135.4</v>
@@ -2501,7 +2553,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1">
         <v>147.30000000000001</v>
@@ -2523,7 +2575,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1">
         <v>154.1</v>
@@ -2545,7 +2597,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1">
         <v>160.5</v>
@@ -2567,7 +2619,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43" s="1">
         <v>184.6</v>
@@ -2589,7 +2641,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1">
         <v>205.3</v>
@@ -2611,7 +2663,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B45" s="1">
         <v>238.3</v>
@@ -2633,7 +2685,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1">
         <v>305</v>
@@ -2652,7 +2704,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B47" s="1">
         <v>90</v>
@@ -2683,7 +2735,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B48" s="19">
         <v>87</v>
@@ -2714,7 +2766,7 @@
     </row>
     <row r="49" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" s="8">
         <v>68.736000000000004</v>

</xml_diff>

<commit_message>
edit reference names of `Lijnen et al., 2001` and `Voros et al., 2005` (mice age -> duration of diet)
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1784E6B0-AE73-614E-9F0C-75AF233E7F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E2E120-5545-3C44-AC37-7BE23F393045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -438,9 +438,6 @@
     <t>Maquoi et al., 2002</t>
   </si>
   <si>
-    <t>Morange et al.,2000</t>
-  </si>
-  <si>
     <t>Lijnen, Maquoi et al., 2003</t>
   </si>
   <si>
@@ -606,19 +603,22 @@
     <t>Cuthbertson &amp; Mandel, 1986 (1.5 mo. Balb/c mice &amp; Retina, Mid-zone)</t>
   </si>
   <si>
-    <t>Voros et al., 2005 (15 wk. mice)</t>
-  </si>
-  <si>
-    <t>Lijnen et al., 2001 (22 wk. mice)</t>
-  </si>
-  <si>
-    <t>Lijnen et al., 2001 (37 wk. mice)</t>
-  </si>
-  <si>
-    <t>Voros et al., 2005 (7 wk. mice)</t>
-  </si>
-  <si>
-    <t>Voros et al., 2005 (10 wk. mice)</t>
+    <t>Lijnen et al., 2001 (17 wk. diet)</t>
+  </si>
+  <si>
+    <t>Lijnen et al., 2001 (32 wk. diet)</t>
+  </si>
+  <si>
+    <t>Morange et al., 2000</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (2 wk. diet)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (5 wk. diet)</t>
+  </si>
+  <si>
+    <t>Voros et al., 2005 (15 wk. diet)</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1272,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1">
         <v>49</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="B6" s="1">
         <v>49</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1">
         <v>21.41</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1">
         <v>26.94</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B9" s="1">
         <v>28.76813695875796</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>62</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <v>40.049999999999997</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="8">
         <v>42.4</v>
@@ -1691,7 +1691,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>3</v>
@@ -1703,7 +1703,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>5</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="21">
         <v>50</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2">
         <v>59</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2">
         <v>75</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2">
         <v>108</v>
@@ -1799,7 +1799,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2">
         <v>154</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="2">
         <v>55</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="2">
         <v>77</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="2">
         <v>158</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="2">
         <v>41</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="2">
         <v>64</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <v>91</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1">
         <v>56.78</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1">
         <v>107.53</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1">
         <v>73</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1">
         <v>92.87</v>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="1">
         <v>76.75</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1">
         <v>178.16</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1">
         <v>67.989999999999995</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1">
         <v>54.75</v>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1">
         <v>103.54</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1">
         <v>78.58</v>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="1">
         <v>63.13</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1">
         <v>56.92</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
         <v>58.75</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1">
         <v>107.62</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1">
         <v>224.2</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1">
         <v>48.5</v>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1">
         <v>61.87</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1">
         <v>55.67</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1">
         <v>93.6</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1">
         <v>108.78</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1">
         <v>89</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1">
         <v>50.8</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1">
         <v>81</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1">
         <v>235.57</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1">
         <v>119</v>
@@ -2509,7 +2509,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1">
         <v>129.1</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1">
         <v>135.4</v>
@@ -2553,7 +2553,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1">
         <v>147.30000000000001</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1">
         <v>154.1</v>
@@ -2597,7 +2597,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1">
         <v>160.5</v>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1">
         <v>184.6</v>
@@ -2641,7 +2641,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1">
         <v>205.3</v>
@@ -2663,7 +2663,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1">
         <v>238.3</v>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1">
         <v>305</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1">
         <v>90</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" s="19">
         <v>87</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="49" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="8">
         <v>68.736000000000004</v>

</xml_diff>

<commit_message>
fix typo in Saito et al., 2003 (LEFT rats -> LETO rats)
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E2E120-5545-3C44-AC37-7BE23F393045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD2A92E-83E8-F442-B832-D74FC5124F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -534,15 +534,9 @@
     <t>Fox et al., 1977 (17 mo. Wistar rat &amp; Kidney)</t>
   </si>
   <si>
-    <t>Saito et al., 2003 (5.5 mo. LEFT rat &amp; Heart)</t>
-  </si>
-  <si>
     <t>Begieneman et al., 2009 (Rat &amp; Heart)</t>
   </si>
   <si>
-    <t>Saito et al., 2003 (15.5 mo. LEFT rat &amp; Heart)</t>
-  </si>
-  <si>
     <t>Ceafalan et al., 2019 (6 mo. C57Bl/6J mice &amp; Brain)</t>
   </si>
   <si>
@@ -619,6 +613,12 @@
   </si>
   <si>
     <t>Voros et al., 2005 (15 wk. diet)</t>
+  </si>
+  <si>
+    <t>Saito et al., 2003 (5.5 mo. LETO rat &amp; Heart)</t>
+  </si>
+  <si>
+    <t>Saito et al., 2003 (15.5 mo. LETO rat &amp; Heart)</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C9A479-2AA3-884B-8FF7-FA729F57839B}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1">
         <v>49</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1">
         <v>49</v>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1">
         <v>21.41</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="1">
         <v>26.94</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="1">
         <v>28.76813695875796</v>
@@ -1669,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="21">
         <v>50</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2">
         <v>59</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2">
         <v>75</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2">
         <v>108</v>
@@ -1799,7 +1799,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2">
         <v>154</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" s="2">
         <v>55</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2">
         <v>77</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2">
         <v>158</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" s="2">
         <v>41</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" s="2">
         <v>64</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1">
         <v>56.78</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1">
         <v>107.53</v>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1">
         <v>76.75</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1">
         <v>54.75</v>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1">
         <v>63.13</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1">
         <v>56.92</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B28" s="1">
         <v>48.5</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1">
         <v>93.6</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1">
         <v>108.78</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B35" s="1">
         <v>81</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B47" s="1">
         <v>90</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B48" s="19">
         <v>87</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="49" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="8">
         <v>68.736000000000004</v>

</xml_diff>

<commit_message>
update CBM thickness data (add additional data extracted from references in review papers)
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD2A92E-83E8-F442-B832-D74FC5124F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BE060A-1D95-4141-A4B3-8203752FE3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -270,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{5B8BC328-C175-1645-944D-85396FC5B1C5}">
+    <comment ref="C45" authorId="0" shapeId="0" xr:uid="{5B8BC328-C175-1645-944D-85396FC5B1C5}">
       <text>
         <r>
           <rPr>
@@ -333,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
+    <comment ref="G45" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
       <text>
         <r>
           <rPr>
@@ -391,7 +391,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -619,6 +619,126 @@
   </si>
   <si>
     <t>Saito et al., 2003 (15.5 mo. LETO rat &amp; Heart)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (2 mo. C57Bl/6 mice &amp; Brain, Striatum)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (2 mo. C57Bl/6 mice &amp; Brain, Cortex)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (2 mo. C57Bl/6 mice &amp; Brain, Hippocampus)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (2 mo. C57Bl/6 mice &amp; Brain, Thalamus)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (7 mo. C57Bl/6 mice &amp; Brain, Striatum)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (7 mo. C57Bl/6 mice &amp; Brain, Cortex)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (7 mo. C57Bl/6 mice &amp; Brain, Hippocampus)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (7 mo. C57Bl/6 mice &amp; Brain, Thalamus)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (23 mo. C57Bl/6 mice &amp; Brain, Striatum)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (23 mo. C57Bl/6 mice &amp; Brain, Cortex)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (23 mo. C57Bl/6 mice &amp; Brain, Hippocampus)</t>
+  </si>
+  <si>
+    <t>Hawkes et al., 2013 (23 mo. C57Bl/6 mice &amp; Brain, Thalamus)</t>
+  </si>
+  <si>
+    <t>Das et al., 1990 (10.5 mo. Wistar rat &amp; Retina, Inner nuclear)</t>
+  </si>
+  <si>
+    <t>Das et al., 1990 (10.5 mo. Wistar rat &amp; Retina, Nerve fiber)</t>
+  </si>
+  <si>
+    <t>Robison et al., 1983 (7 mo. Sprague-Dawley rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Robison et al., 1983 (11 mo. Sprague-Dawley rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Roy et al., 2003 (7 mo. Sprague-Dawley rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Dosso et al., 2004 (7 mo. Wistar rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Evans et al., 2000 (6 mo. Sprague-Dawley rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Zheng et al., 2007 (8 mo. Sprague-Dawley rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Frank et al., 1983 (6 mo. Wistar rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Frank et al., 1983 (9 mo. Wistar rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Frank et al., 1983 (12 mo. Wistar rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Frank et al., 1983 (19.5 mo. Wistar rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>McCaleb et al., 1991 (10.5 mo. Wistar rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Smith et al., 1995 (6 mo. Sprague-Dawley rat &amp; Inner ear)</t>
+  </si>
+  <si>
+    <t>Robison et al., 1986 (7 mo. Sprague-Dawley rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Clements et al., 1998 (5.5 mo. db/m rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Sima et al., 1988 (4 mo. Lewis rat &amp; Retina, Superficial capillary)</t>
+  </si>
+  <si>
+    <t>Chakrabarti &amp; Sima, 1989 (7 mo. BB rat &amp; Retina, Superficial capillary)</t>
+  </si>
+  <si>
+    <t>Chakrabarti &amp; Sima, 1989 (7 mo. BB rat &amp; Retina, Deep capillary)</t>
+  </si>
+  <si>
+    <t>Sima et al., 1988 (4 mo. Lewis rat &amp; Retina, Deep capillary)</t>
+  </si>
+  <si>
+    <t>Kern &amp; Engerman, 1994 (20 mo. Sprague-Dawley rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Chakrabarti et al., 1991 (6 mo. BB rat &amp; Retina, Superficial capillary)</t>
+  </si>
+  <si>
+    <t>Chakrabarti et al., 1991 (6 mo. BB rat &amp; Retina, Deep capillary)</t>
+  </si>
+  <si>
+    <t>Chakrabarti et al., 1991 (6 mo. BB rat &amp; Muscle)</t>
+  </si>
+  <si>
+    <t>Chakrabarti et al., 1991 (6 mo. BB rat &amp; Endoneurial capillary)</t>
+  </si>
+  <si>
+    <t>Chakrabarti et al., 1991 (6 mo. BB rat &amp; Kidney)</t>
+  </si>
+  <si>
+    <t>Roy et al., 2011 (6 mo. Sprague-Dawley rat &amp; Retina)</t>
+  </si>
+  <si>
+    <t>Li et al., 2018 (8 mo. Sprague-Dawley rat &amp; Retina)</t>
   </si>
 </sst>
 </file>
@@ -662,7 +782,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -909,11 +1029,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -951,10 +1108,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,9 +1137,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1013,7 +1177,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1119,7 +1283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1261,7 +1425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1329,7 +1493,7 @@
       <c r="E2" s="6">
         <v>1.838396591281048</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1364,7 +1528,7 @@
       <c r="E3" s="7">
         <v>5.3</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1397,7 +1561,7 @@
       <c r="E4" s="7">
         <v>1.6</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1432,7 +1596,7 @@
       <c r="E5" s="7">
         <v>3</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="25" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1467,7 +1631,7 @@
       <c r="E6" s="7">
         <v>3.5</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1504,7 +1668,7 @@
       <c r="E7" s="7">
         <v>0.72</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1667,10 +1831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2305,96 +2469,74 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1">
-        <v>61.87</v>
+        <v>67.03</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E29" s="1">
-        <v>1.33</v>
-      </c>
-      <c r="F29" s="1">
-        <v>68.13</v>
-      </c>
+        <v>4.34</v>
+      </c>
+      <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1">
-        <v>6</v>
-      </c>
-      <c r="I29" s="7">
-        <v>1.66</v>
-      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="B30" s="1">
-        <v>55.67</v>
+        <v>65.790000000000006</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
-        <v>6</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1.04</v>
-      </c>
-      <c r="F30" s="1">
-        <v>57.82</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E30" s="26">
+        <v>5.56</v>
+      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1">
-        <v>7</v>
-      </c>
-      <c r="I30" s="7">
-        <v>1.24</v>
-      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B31" s="1">
-        <v>93.6</v>
-      </c>
-      <c r="C31" s="1">
-        <v>6.12</v>
-      </c>
+        <v>62.58</v>
+      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E31" s="1">
-        <f>C31/SQRT(D31)</f>
-        <v>2.7369472044597427</v>
-      </c>
-      <c r="F31" s="1">
-        <v>104.6</v>
-      </c>
-      <c r="G31" s="1">
-        <v>4.58</v>
-      </c>
-      <c r="H31" s="1">
-        <v>4</v>
-      </c>
-      <c r="I31" s="7">
-        <f>G31/SQRT(H31)</f>
-        <v>2.29</v>
-      </c>
+        <v>2.7</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="B32" s="1">
-        <v>108.78</v>
+        <v>70.11</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="D32" s="1">
+        <v>3</v>
+      </c>
       <c r="E32" s="1">
-        <v>11.2</v>
+        <v>3.63</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2403,43 +2545,36 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1">
-        <v>89</v>
+        <v>74.94</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
       <c r="E33" s="1">
-        <f>B33*2.2/100</f>
-        <v>1.9580000000000002</v>
-      </c>
-      <c r="F33" s="1">
-        <v>113.4</v>
-      </c>
+        <v>6.62</v>
+      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="7">
-        <f>B33*2/100</f>
-        <v>1.78</v>
-      </c>
+      <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B34" s="1">
-        <v>50.8</v>
-      </c>
-      <c r="C34" s="1">
-        <v>5.0999999999999996</v>
-      </c>
+        <v>57.35</v>
+      </c>
+      <c r="C34" s="1"/>
       <c r="D34" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E34" s="1">
-        <f>C34/SQRT(D34)</f>
-        <v>2.0820662813657016</v>
+        <v>4.33</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2448,20 +2583,17 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B35" s="1">
-        <v>81</v>
-      </c>
-      <c r="C35" s="1">
-        <v>9.9</v>
-      </c>
+        <v>63.5</v>
+      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E35" s="1">
-        <f>C35/SQRT(D35)</f>
-        <v>4.0416580755922444</v>
+        <v>4.78</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2470,15 +2602,17 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="B36" s="1">
-        <v>235.57</v>
+        <v>58.62</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="D36" s="1">
+        <v>3</v>
+      </c>
       <c r="E36" s="1">
-        <v>1.05</v>
+        <v>5.17</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -2486,21 +2620,18 @@
       <c r="I36" s="7"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>37</v>
+      <c r="A37" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="B37" s="1">
-        <v>119</v>
-      </c>
-      <c r="C37" s="1">
-        <v>6.8</v>
-      </c>
+        <v>74.23</v>
+      </c>
+      <c r="C37" s="1"/>
       <c r="D37" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E37" s="1">
-        <f>C37/SQRT(D37)</f>
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -2508,21 +2639,18 @@
       <c r="I37" s="7"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>38</v>
+      <c r="A38" s="20" t="s">
+        <v>85</v>
       </c>
       <c r="B38" s="1">
-        <v>129.1</v>
-      </c>
-      <c r="C38" s="1">
-        <v>4.5999999999999996</v>
-      </c>
+        <v>97.49</v>
+      </c>
+      <c r="C38" s="1"/>
       <c r="D38" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" ref="E38:E48" si="1">C38/SQRT(D38)</f>
-        <v>2.2999999999999998</v>
+        <v>12.27</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2530,21 +2658,18 @@
       <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>39</v>
+      <c r="A39" s="20" t="s">
+        <v>86</v>
       </c>
       <c r="B39" s="1">
-        <v>135.4</v>
-      </c>
-      <c r="C39" s="1">
-        <v>3.5</v>
-      </c>
+        <v>109.5</v>
+      </c>
+      <c r="C39" s="1"/>
       <c r="D39" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E39" s="1">
-        <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>11.93</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -2552,21 +2677,18 @@
       <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>40</v>
+      <c r="A40" s="20" t="s">
+        <v>87</v>
       </c>
       <c r="B40" s="1">
-        <v>147.30000000000001</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1.3</v>
-      </c>
+        <v>108.43</v>
+      </c>
+      <c r="C40" s="1"/>
       <c r="D40" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E40" s="1">
-        <f t="shared" si="1"/>
-        <v>0.65</v>
+        <v>14.51</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2575,86 +2697,96 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B41" s="1">
-        <v>154.1</v>
-      </c>
-      <c r="C41" s="1">
-        <v>3.5</v>
-      </c>
+        <v>61.87</v>
+      </c>
+      <c r="C41" s="1"/>
       <c r="D41" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E41" s="1">
-        <f t="shared" si="1"/>
-        <v>1.75</v>
-      </c>
-      <c r="F41" s="1"/>
+        <v>1.33</v>
+      </c>
+      <c r="F41" s="1">
+        <v>68.13</v>
+      </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="7"/>
+      <c r="H41" s="1">
+        <v>6</v>
+      </c>
+      <c r="I41" s="7">
+        <v>1.66</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B42" s="1">
-        <v>160.5</v>
-      </c>
-      <c r="C42" s="1">
-        <v>3.8</v>
-      </c>
+        <v>55.67</v>
+      </c>
+      <c r="C42" s="1"/>
       <c r="D42" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E42" s="1">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>1.04</v>
+      </c>
+      <c r="F42" s="1">
+        <v>57.82</v>
+      </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="7"/>
+      <c r="H42" s="1">
+        <v>7</v>
+      </c>
+      <c r="I42" s="7">
+        <v>1.24</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B43" s="1">
-        <v>184.6</v>
+        <v>93.6</v>
       </c>
       <c r="C43" s="1">
-        <v>6.5</v>
+        <v>6.12</v>
       </c>
       <c r="D43" s="1">
+        <v>5</v>
+      </c>
+      <c r="E43" s="1">
+        <f>C43/SQRT(D43)</f>
+        <v>2.7369472044597427</v>
+      </c>
+      <c r="F43" s="1">
+        <v>104.6</v>
+      </c>
+      <c r="G43" s="1">
+        <v>4.58</v>
+      </c>
+      <c r="H43" s="1">
         <v>4</v>
       </c>
-      <c r="E43" s="1">
-        <f t="shared" si="1"/>
-        <v>3.25</v>
-      </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="7"/>
+      <c r="I43" s="7">
+        <f>G43/SQRT(H43)</f>
+        <v>2.29</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="23" t="s">
-        <v>44</v>
+      <c r="A44" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B44" s="1">
-        <v>205.3</v>
-      </c>
-      <c r="C44" s="1">
-        <v>7.2</v>
-      </c>
-      <c r="D44" s="1">
-        <v>4</v>
-      </c>
+        <v>108.78</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
       <c r="E44" s="1">
-        <f t="shared" si="1"/>
-        <v>3.6</v>
+        <v>11.2</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -2662,40 +2794,44 @@
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="23" t="s">
-        <v>45</v>
+      <c r="A45" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="B45" s="1">
-        <v>238.3</v>
-      </c>
-      <c r="C45" s="1">
-        <v>11.4</v>
-      </c>
-      <c r="D45" s="1">
-        <v>4</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
       <c r="E45" s="1">
-        <f t="shared" si="1"/>
-        <v>5.7</v>
-      </c>
-      <c r="F45" s="1"/>
+        <f>B45*2.2/100</f>
+        <v>1.9580000000000002</v>
+      </c>
+      <c r="F45" s="1">
+        <v>113.4</v>
+      </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="7"/>
+      <c r="I45" s="7">
+        <f>B45*2/100</f>
+        <v>1.78</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B46" s="1">
-        <v>305</v>
-      </c>
-      <c r="C46" s="1"/>
+        <v>50.8</v>
+      </c>
+      <c r="C46" s="1">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="D46" s="1">
         <v>6</v>
       </c>
       <c r="E46" s="1">
-        <v>10</v>
+        <f>C46/SQRT(D46)</f>
+        <v>2.0820662813657016</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -2704,84 +2840,900 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="1">
+        <v>81</v>
+      </c>
+      <c r="C47" s="1">
+        <v>9.9</v>
+      </c>
+      <c r="D47" s="1">
+        <v>6</v>
+      </c>
+      <c r="E47" s="1">
+        <f>C47/SQRT(D47)</f>
+        <v>4.0416580755922444</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="7"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="1">
+        <v>235.57</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="1">
+        <v>119</v>
+      </c>
+      <c r="C49" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="D49" s="1">
+        <v>4</v>
+      </c>
+      <c r="E49" s="1">
+        <f>C49/SQRT(D49)</f>
+        <v>3.4</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="1">
+        <v>129.1</v>
+      </c>
+      <c r="C50" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D50" s="1">
+        <v>4</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" ref="E50:E60" si="1">C50/SQRT(D50)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="7"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="1">
+        <v>135.4</v>
+      </c>
+      <c r="C51" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D51" s="1">
+        <v>4</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="7"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="1">
+        <v>147.30000000000001</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="D52" s="1">
+        <v>4</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="1">
+        <v>154.1</v>
+      </c>
+      <c r="C53" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D53" s="1">
+        <v>4</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="1">
+        <v>160.5</v>
+      </c>
+      <c r="C54" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="D54" s="1">
+        <v>4</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="7"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="1">
+        <v>184.6</v>
+      </c>
+      <c r="C55" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="D55" s="1">
+        <v>4</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="1"/>
+        <v>3.25</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="1">
+        <v>205.3</v>
+      </c>
+      <c r="C56" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="D56" s="1">
+        <v>4</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="7"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="1">
+        <v>238.3</v>
+      </c>
+      <c r="C57" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="D57" s="1">
+        <v>4</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="1"/>
+        <v>5.7</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="7"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" s="1">
+        <v>305</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1">
+        <v>6</v>
+      </c>
+      <c r="E58" s="1">
+        <v>10</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="7"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B59" s="1">
         <v>90</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C59" s="1">
         <v>12</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D59" s="1">
         <v>50</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E59" s="1">
         <f t="shared" si="1"/>
         <v>1.697056274847714</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F59" s="1">
         <v>106</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G59" s="1">
         <v>20</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H59" s="1">
         <v>50</v>
       </c>
-      <c r="I47" s="7">
-        <f>G47/SQRT(H47)</f>
+      <c r="I59" s="7">
+        <f>G59/SQRT(H59)</f>
         <v>2.8284271247461898</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="19">
+      <c r="B60" s="19">
         <v>87</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C60" s="19">
         <v>12</v>
       </c>
-      <c r="D48" s="19">
+      <c r="D60" s="19">
         <v>50</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E60" s="1">
         <f t="shared" si="1"/>
         <v>1.697056274847714</v>
       </c>
-      <c r="F48" s="19">
+      <c r="F60" s="19">
         <v>177</v>
       </c>
-      <c r="G48" s="19">
+      <c r="G60" s="19">
         <v>66</v>
       </c>
-      <c r="H48" s="19">
+      <c r="H60" s="19">
         <v>50</v>
       </c>
-      <c r="I48" s="7">
-        <f>G48/SQRT(H48)</f>
+      <c r="I60" s="7">
+        <f>G60/SQRT(H60)</f>
         <v>9.3338095116624267</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B61" s="19">
         <v>68.736000000000004</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8">
+      <c r="C61" s="19"/>
+      <c r="D61" s="19">
         <v>6</v>
       </c>
-      <c r="E49" s="8">
+      <c r="E61" s="19">
         <v>4.22</v>
       </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="9"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="28"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" s="29">
+        <v>166.7</v>
+      </c>
+      <c r="C62" s="29">
+        <v>44.5</v>
+      </c>
+      <c r="D62" s="29">
+        <v>5</v>
+      </c>
+      <c r="E62" s="1">
+        <f>C62/SQRT(D62)</f>
+        <v>19.901004999748128</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="7"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="29">
+        <v>206.5</v>
+      </c>
+      <c r="C63" s="29">
+        <v>42.3</v>
+      </c>
+      <c r="D63" s="29">
+        <v>5</v>
+      </c>
+      <c r="E63" s="1">
+        <f>C63/SQRT(D63)</f>
+        <v>18.91713508964822</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="7"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="29">
+        <v>96.7</v>
+      </c>
+      <c r="C64" s="29">
+        <v>14.1</v>
+      </c>
+      <c r="D64" s="29">
+        <v>3</v>
+      </c>
+      <c r="E64" s="29">
+        <f>C64/SQRT(D64)</f>
+        <v>8.1406387955737234</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="7"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" s="29">
+        <v>93.9</v>
+      </c>
+      <c r="C65" s="29">
+        <v>12.3</v>
+      </c>
+      <c r="D65" s="29">
+        <v>3</v>
+      </c>
+      <c r="E65" s="29">
+        <f>C65/SQRT(D65)</f>
+        <v>7.1014083110323973</v>
+      </c>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="7"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B66" s="29">
+        <v>85</v>
+      </c>
+      <c r="C66" s="29">
+        <v>20</v>
+      </c>
+      <c r="D66" s="29">
+        <v>5</v>
+      </c>
+      <c r="E66" s="29">
+        <f>C66/SQRT(D66)</f>
+        <v>8.9442719099991592</v>
+      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="7"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" s="29">
+        <v>66.141999999999996</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="29">
+        <v>8</v>
+      </c>
+      <c r="E67" s="1">
+        <v>2.7559999999999998</v>
+      </c>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="7"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="29">
+        <v>75.658000000000001</v>
+      </c>
+      <c r="C68" s="1">
+        <v>10.526</v>
+      </c>
+      <c r="D68" s="29">
+        <v>8</v>
+      </c>
+      <c r="E68" s="1">
+        <f>C68/SQRT(D68)</f>
+        <v>3.7215029893847995</v>
+      </c>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="7"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B69" s="29">
+        <v>111.8</v>
+      </c>
+      <c r="C69" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="D69" s="29">
+        <v>7</v>
+      </c>
+      <c r="E69" s="29">
+        <f>C69/SQRT(D69)</f>
+        <v>5.3670955167310259</v>
+      </c>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="7"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B70" s="29">
+        <v>81.58</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="29">
+        <v>4</v>
+      </c>
+      <c r="E70" s="1">
+        <v>7.89</v>
+      </c>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="7"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B71" s="29">
+        <v>94.74</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="29">
+        <v>4</v>
+      </c>
+      <c r="E71" s="1">
+        <v>7.89</v>
+      </c>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="7"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" s="29">
+        <v>121.05</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="29">
+        <v>4</v>
+      </c>
+      <c r="E72" s="1">
+        <v>19.3</v>
+      </c>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="7"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B73" s="29">
+        <v>160.4</v>
+      </c>
+      <c r="C73" s="1">
+        <v>31.2</v>
+      </c>
+      <c r="D73" s="29">
+        <v>7</v>
+      </c>
+      <c r="E73" s="1">
+        <f>C73/SQRT(D73)</f>
+        <v>11.792491557887889</v>
+      </c>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="7"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" s="29">
+        <v>134.6</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="29">
+        <v>5</v>
+      </c>
+      <c r="E74" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="7"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B75" s="29">
+        <v>95.1</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="29">
+        <v>5</v>
+      </c>
+      <c r="E75" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="7"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B76" s="29">
+        <v>84.403000000000006</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="29">
+        <v>6</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1.1619999999999999</v>
+      </c>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="7"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" s="29">
+        <v>102</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1">
+        <v>9</v>
+      </c>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="7"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" s="29">
+        <v>122.9</v>
+      </c>
+      <c r="C78" s="1">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="D78" s="1">
+        <v>4</v>
+      </c>
+      <c r="E78" s="1">
+        <f>C78/SQRT(D78)</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="7"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B79" s="29">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="7"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" s="29">
+        <v>146.19999999999999</v>
+      </c>
+      <c r="C80" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="D80" s="1">
+        <v>5</v>
+      </c>
+      <c r="E80" s="1">
+        <f>C80/SQRT(D80)</f>
+        <v>2.996331089849718</v>
+      </c>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="7"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="29">
+        <v>97.4</v>
+      </c>
+      <c r="C81" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="D81" s="1">
+        <v>5</v>
+      </c>
+      <c r="E81" s="1">
+        <f>C81/SQRT(D81)</f>
+        <v>3.3541019662496843</v>
+      </c>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="7"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B82" s="29">
+        <v>159</v>
+      </c>
+      <c r="C82" s="1">
+        <v>23</v>
+      </c>
+      <c r="D82" s="1">
+        <v>13</v>
+      </c>
+      <c r="E82" s="1">
+        <f>C82/SQRT(D82)</f>
+        <v>6.3790522565901355</v>
+      </c>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="7"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83" s="29">
+        <v>161.9</v>
+      </c>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="7"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" s="29">
+        <v>142.69999999999999</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="7"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" s="29">
+        <v>125</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="7"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B86" s="29">
+        <v>142.80000000000001</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="7"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B87" s="29">
+        <v>326</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1">
+        <v>20</v>
+      </c>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="7"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B88" s="29">
+        <v>51.5</v>
+      </c>
+      <c r="C88" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="D88" s="1">
+        <v>8</v>
+      </c>
+      <c r="E88" s="1">
+        <f>C88/SQRT(D88)</f>
+        <v>1.6970562748477138</v>
+      </c>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="7"/>
+    </row>
+    <row r="89" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B89" s="33">
+        <v>94.6</v>
+      </c>
+      <c r="C89" s="8">
+        <v>7.7</v>
+      </c>
+      <c r="D89" s="8">
+        <v>6</v>
+      </c>
+      <c r="E89" s="8">
+        <f>C89/SQRT(D89)</f>
+        <v>3.1435118365717454</v>
+      </c>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update the number of significant digits
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BE060A-1D95-4141-A4B3-8203752FE3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A376CE-0769-B947-9818-B4C7E78279F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -1070,7 +1070,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1108,17 +1108,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1435,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C9A479-2AA3-884B-8FF7-FA729F57839B}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1482,18 +1478,18 @@
         <v>13</v>
       </c>
       <c r="B2" s="2">
-        <v>44.993898209967412</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2">
-        <v>2.5468244269792875</v>
+        <v>2.5</v>
       </c>
       <c r="D2" s="2">
-        <v>65.795246424795408</v>
+        <v>66</v>
       </c>
       <c r="E2" s="6">
-        <v>1.838396591281048</v>
-      </c>
-      <c r="G2" s="25" t="s">
+        <v>1.8</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1528,7 +1524,7 @@
       <c r="E3" s="7">
         <v>5.3</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1561,7 +1557,7 @@
       <c r="E4" s="7">
         <v>1.6</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1596,7 +1592,7 @@
       <c r="E5" s="7">
         <v>3</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="29" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1631,7 +1627,7 @@
       <c r="E6" s="7">
         <v>3.5</v>
       </c>
-      <c r="G6" s="25"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1657,18 +1653,18 @@
         <v>71</v>
       </c>
       <c r="B7" s="1">
-        <v>21.41</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
         <v>0.83</v>
       </c>
       <c r="D7" s="1">
-        <v>34.6</v>
+        <v>35</v>
       </c>
       <c r="E7" s="7">
         <v>0.72</v>
       </c>
-      <c r="G7" s="25"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1694,13 +1690,13 @@
         <v>72</v>
       </c>
       <c r="B8" s="1">
-        <v>26.94</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
         <v>0.47</v>
       </c>
       <c r="D8" s="1">
-        <v>40.68</v>
+        <v>41</v>
       </c>
       <c r="E8" s="7">
         <v>2.0299999999999998</v>
@@ -1711,16 +1707,16 @@
         <v>73</v>
       </c>
       <c r="B9" s="1">
-        <v>28.76813695875796</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1">
-        <v>1.0622081338618323</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D9" s="1">
-        <v>52.925674284012274</v>
+        <v>53</v>
       </c>
       <c r="E9" s="7">
-        <v>0.45708536881646961</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1748,16 +1744,16 @@
         <v>16</v>
       </c>
       <c r="B11" s="1">
-        <v>40.049999999999997</v>
+        <v>40.1</v>
       </c>
       <c r="C11" s="1">
         <v>0.76</v>
       </c>
       <c r="D11" s="1">
-        <v>94.61</v>
+        <v>94.6</v>
       </c>
       <c r="E11" s="7">
-        <v>4.58</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1767,10 +1763,10 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
-        <v>76.36</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="E12" s="7">
-        <v>2.25</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I12">
         <f>SQRT((I5+J5)/PI())*2</f>
@@ -1788,7 +1784,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
-        <v>89.13</v>
+        <v>89.1</v>
       </c>
       <c r="E13" s="7">
         <v>1.46</v>
@@ -1833,7 +1829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
@@ -2497,7 +2493,7 @@
       <c r="D30" s="1">
         <v>3</v>
       </c>
-      <c r="E30" s="26">
+      <c r="E30" s="25">
         <v>5.56</v>
       </c>
       <c r="F30" s="1"/>
@@ -3157,7 +3153,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="27" t="s">
+      <c r="A61" s="26" t="s">
         <v>47</v>
       </c>
       <c r="B61" s="19">
@@ -3173,19 +3169,19 @@
       <c r="F61" s="19"/>
       <c r="G61" s="19"/>
       <c r="H61" s="19"/>
-      <c r="I61" s="28"/>
+      <c r="I61" s="27"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="30" t="s">
+      <c r="A62" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B62" s="29">
+      <c r="B62" s="1">
         <v>166.7</v>
       </c>
-      <c r="C62" s="29">
+      <c r="C62" s="1">
         <v>44.5</v>
       </c>
-      <c r="D62" s="29">
+      <c r="D62" s="1">
         <v>5</v>
       </c>
       <c r="E62" s="1">
@@ -3198,16 +3194,16 @@
       <c r="I62" s="7"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="30" t="s">
+      <c r="A63" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B63" s="29">
+      <c r="B63" s="1">
         <v>206.5</v>
       </c>
-      <c r="C63" s="29">
+      <c r="C63" s="1">
         <v>42.3</v>
       </c>
-      <c r="D63" s="29">
+      <c r="D63" s="1">
         <v>5</v>
       </c>
       <c r="E63" s="1">
@@ -3220,19 +3216,19 @@
       <c r="I63" s="7"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="30" t="s">
+      <c r="A64" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B64" s="29">
+      <c r="B64" s="1">
         <v>96.7</v>
       </c>
-      <c r="C64" s="29">
+      <c r="C64" s="1">
         <v>14.1</v>
       </c>
-      <c r="D64" s="29">
+      <c r="D64" s="1">
         <v>3</v>
       </c>
-      <c r="E64" s="29">
+      <c r="E64" s="1">
         <f>C64/SQRT(D64)</f>
         <v>8.1406387955737234</v>
       </c>
@@ -3242,19 +3238,19 @@
       <c r="I64" s="7"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="30" t="s">
+      <c r="A65" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B65" s="29">
+      <c r="B65" s="1">
         <v>93.9</v>
       </c>
-      <c r="C65" s="29">
+      <c r="C65" s="1">
         <v>12.3</v>
       </c>
-      <c r="D65" s="29">
+      <c r="D65" s="1">
         <v>3</v>
       </c>
-      <c r="E65" s="29">
+      <c r="E65" s="1">
         <f>C65/SQRT(D65)</f>
         <v>7.1014083110323973</v>
       </c>
@@ -3264,19 +3260,19 @@
       <c r="I65" s="7"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="30" t="s">
+      <c r="A66" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B66" s="29">
+      <c r="B66" s="1">
         <v>85</v>
       </c>
-      <c r="C66" s="29">
+      <c r="C66" s="1">
         <v>20</v>
       </c>
-      <c r="D66" s="29">
+      <c r="D66" s="1">
         <v>5</v>
       </c>
-      <c r="E66" s="29">
+      <c r="E66" s="1">
         <f>C66/SQRT(D66)</f>
         <v>8.9442719099991592</v>
       </c>
@@ -3286,14 +3282,14 @@
       <c r="I66" s="7"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="30" t="s">
+      <c r="A67" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B67" s="29">
+      <c r="B67" s="1">
         <v>66.141999999999996</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="29">
+      <c r="D67" s="1">
         <v>8</v>
       </c>
       <c r="E67" s="1">
@@ -3305,16 +3301,16 @@
       <c r="I67" s="7"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="30" t="s">
+      <c r="A68" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B68" s="29">
+      <c r="B68" s="1">
         <v>75.658000000000001</v>
       </c>
       <c r="C68" s="1">
         <v>10.526</v>
       </c>
-      <c r="D68" s="29">
+      <c r="D68" s="1">
         <v>8</v>
       </c>
       <c r="E68" s="1">
@@ -3327,19 +3323,19 @@
       <c r="I68" s="7"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="30" t="s">
+      <c r="A69" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B69" s="29">
+      <c r="B69" s="1">
         <v>111.8</v>
       </c>
       <c r="C69" s="1">
         <v>14.2</v>
       </c>
-      <c r="D69" s="29">
+      <c r="D69" s="1">
         <v>7</v>
       </c>
-      <c r="E69" s="29">
+      <c r="E69" s="1">
         <f>C69/SQRT(D69)</f>
         <v>5.3670955167310259</v>
       </c>
@@ -3349,14 +3345,14 @@
       <c r="I69" s="7"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="30" t="s">
+      <c r="A70" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B70" s="29">
+      <c r="B70" s="1">
         <v>81.58</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="D70" s="29">
+      <c r="D70" s="1">
         <v>4</v>
       </c>
       <c r="E70" s="1">
@@ -3368,14 +3364,14 @@
       <c r="I70" s="7"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="30" t="s">
+      <c r="A71" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B71" s="29">
+      <c r="B71" s="1">
         <v>94.74</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="29">
+      <c r="D71" s="1">
         <v>4</v>
       </c>
       <c r="E71" s="1">
@@ -3390,11 +3386,11 @@
       <c r="A72" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B72" s="29">
+      <c r="B72" s="1">
         <v>121.05</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="29">
+      <c r="D72" s="1">
         <v>4</v>
       </c>
       <c r="E72" s="1">
@@ -3406,16 +3402,16 @@
       <c r="I72" s="7"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="30" t="s">
+      <c r="A73" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B73" s="29">
+      <c r="B73" s="1">
         <v>160.4</v>
       </c>
       <c r="C73" s="1">
         <v>31.2</v>
       </c>
-      <c r="D73" s="29">
+      <c r="D73" s="1">
         <v>7</v>
       </c>
       <c r="E73" s="1">
@@ -3428,14 +3424,14 @@
       <c r="I73" s="7"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="30" t="s">
+      <c r="A74" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B74" s="29">
+      <c r="B74" s="1">
         <v>134.6</v>
       </c>
       <c r="C74" s="1"/>
-      <c r="D74" s="29">
+      <c r="D74" s="1">
         <v>5</v>
       </c>
       <c r="E74" s="1">
@@ -3447,14 +3443,14 @@
       <c r="I74" s="7"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B75" s="29">
+      <c r="B75" s="1">
         <v>95.1</v>
       </c>
       <c r="C75" s="1"/>
-      <c r="D75" s="29">
+      <c r="D75" s="1">
         <v>5</v>
       </c>
       <c r="E75" s="1">
@@ -3466,14 +3462,14 @@
       <c r="I75" s="7"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" s="30" t="s">
+      <c r="A76" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B76" s="29">
+      <c r="B76" s="1">
         <v>84.403000000000006</v>
       </c>
       <c r="C76" s="1"/>
-      <c r="D76" s="29">
+      <c r="D76" s="1">
         <v>6</v>
       </c>
       <c r="E76" s="1">
@@ -3485,10 +3481,10 @@
       <c r="I76" s="7"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="30" t="s">
+      <c r="A77" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B77" s="29">
+      <c r="B77" s="1">
         <v>102</v>
       </c>
       <c r="C77" s="1"/>
@@ -3502,10 +3498,10 @@
       <c r="I77" s="7"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="30" t="s">
+      <c r="A78" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B78" s="29">
+      <c r="B78" s="1">
         <v>122.9</v>
       </c>
       <c r="C78" s="1">
@@ -3524,10 +3520,10 @@
       <c r="I78" s="7"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="30" t="s">
+      <c r="A79" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B79" s="29">
+      <c r="B79" s="1">
         <v>79.400000000000006</v>
       </c>
       <c r="C79" s="1"/>
@@ -3541,10 +3537,10 @@
       <c r="I79" s="7"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="30" t="s">
+      <c r="A80" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B80" s="29">
+      <c r="B80" s="1">
         <v>146.19999999999999</v>
       </c>
       <c r="C80" s="1">
@@ -3563,10 +3559,10 @@
       <c r="I80" s="7"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="30" t="s">
+      <c r="A81" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B81" s="29">
+      <c r="B81" s="1">
         <v>97.4</v>
       </c>
       <c r="C81" s="1">
@@ -3585,10 +3581,10 @@
       <c r="I81" s="7"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="30" t="s">
+      <c r="A82" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B82" s="29">
+      <c r="B82" s="1">
         <v>159</v>
       </c>
       <c r="C82" s="1">
@@ -3607,10 +3603,10 @@
       <c r="I82" s="7"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="30" t="s">
+      <c r="A83" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B83" s="29">
+      <c r="B83" s="1">
         <v>161.9</v>
       </c>
       <c r="C83" s="1"/>
@@ -3624,10 +3620,10 @@
       <c r="I83" s="7"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="30" t="s">
+      <c r="A84" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B84" s="29">
+      <c r="B84" s="1">
         <v>142.69999999999999</v>
       </c>
       <c r="C84" s="1"/>
@@ -3644,7 +3640,7 @@
       <c r="A85" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B85" s="29">
+      <c r="B85" s="1">
         <v>125</v>
       </c>
       <c r="C85" s="1"/>
@@ -3661,7 +3657,7 @@
       <c r="A86" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="B86" s="29">
+      <c r="B86" s="1">
         <v>142.80000000000001</v>
       </c>
       <c r="C86" s="1"/>
@@ -3678,7 +3674,7 @@
       <c r="A87" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B87" s="29">
+      <c r="B87" s="1">
         <v>326</v>
       </c>
       <c r="C87" s="1"/>
@@ -3692,10 +3688,10 @@
       <c r="I87" s="7"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="31" t="s">
+      <c r="A88" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="B88" s="29">
+      <c r="B88" s="1">
         <v>51.5</v>
       </c>
       <c r="C88" s="1">
@@ -3714,10 +3710,10 @@
       <c r="I88" s="7"/>
     </row>
     <row r="89" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="32" t="s">
+      <c r="A89" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B89" s="33">
+      <c r="B89" s="8">
         <v>94.6</v>
       </c>
       <c r="C89" s="8">

</xml_diff>

<commit_message>
update the number of significant digits to match it with that of mean value
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A376CE-0769-B947-9818-B4C7E78279F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D522A27-189C-0B43-8B75-1FFFD01A550E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="14700" windowHeight="16700" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22400" windowHeight="22760" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -1431,7 +1431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C9A479-2AA3-884B-8FF7-FA729F57839B}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1829,7 +1829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
@@ -1905,7 +1905,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E25" si="0">C3/SQRT(D3)</f>
+        <f t="shared" ref="E3:E14" si="0">C3/SQRT(D3)</f>
         <v>6.5</v>
       </c>
       <c r="F3" s="2"/>
@@ -1993,8 +1993,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>6.3639610306789276</v>
+        <v>6.4</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="18"/>
@@ -2015,8 +2014,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>6.3639610306789276</v>
+        <v>6.4</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="18"/>
@@ -2037,8 +2035,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>24.748737341529161</v>
+        <v>24.7</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="18"/>
@@ -2059,8 +2056,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>2.8284271247461898</v>
+        <v>2.8</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="18"/>
@@ -2081,8 +2077,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
-        <v>4.2426406871192848</v>
+        <v>4.2</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="18"/>
@@ -2103,8 +2098,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>0.86602540378443871</v>
+        <v>0.87</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="18"/>
@@ -2169,8 +2163,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
-        <v>5.6568542494923797</v>
+        <v>5.7</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="18"/>
@@ -2191,8 +2184,7 @@
         <v>8</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>6.6821590822128734</v>
+        <v>6.6820000000000004</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="18"/>
@@ -2213,8 +2205,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
-        <v>4.4809474444585931</v>
+        <v>4.4809999999999999</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="18"/>
@@ -2235,8 +2226,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
-        <v>8.1694942831307031</v>
+        <v>8.1694999999999993</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="18"/>
@@ -2257,8 +2247,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>2.4571960646232527</v>
+        <v>2.4569999999999999</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="18"/>
@@ -2279,8 +2268,7 @@
         <v>8</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7677669529663687</v>
+        <v>1.768</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="18"/>
@@ -2301,8 +2289,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
-        <v>5.77352686838816</v>
+        <v>5.7735000000000003</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="18"/>
@@ -2323,8 +2310,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="0"/>
-        <v>4.0760929004787583</v>
+        <v>4.0759999999999996</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="18"/>
@@ -2345,8 +2331,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7060700454553444</v>
+        <v>1.706</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="18"/>
@@ -2367,8 +2352,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="0"/>
-        <v>1.1604740410711478</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="18"/>
@@ -2389,8 +2373,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
-        <v>2.5458410529070084</v>
+        <v>2.5459999999999998</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="18"/>
@@ -2427,7 +2410,7 @@
         <v>31</v>
       </c>
       <c r="B27" s="1">
-        <v>224.2</v>
+        <v>224</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
@@ -2455,8 +2438,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="1">
-        <f>C28/SQRT(D28)</f>
-        <v>2.762920297697451</v>
+        <v>2.7629999999999999</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -2755,8 +2737,7 @@
         <v>5</v>
       </c>
       <c r="E43" s="1">
-        <f>C43/SQRT(D43)</f>
-        <v>2.7369472044597427</v>
+        <v>2.7370000000000001</v>
       </c>
       <c r="F43" s="1">
         <v>104.6</v>
@@ -2777,7 +2758,7 @@
         <v>51</v>
       </c>
       <c r="B44" s="1">
-        <v>108.78</v>
+        <v>108.8</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2826,8 +2807,7 @@
         <v>6</v>
       </c>
       <c r="E46" s="1">
-        <f>C46/SQRT(D46)</f>
-        <v>2.0820662813657016</v>
+        <v>2.08</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -2848,8 +2828,7 @@
         <v>6</v>
       </c>
       <c r="E47" s="1">
-        <f>C47/SQRT(D47)</f>
-        <v>4.0416580755922444</v>
+        <v>4.04</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -2909,7 +2888,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="1">
-        <f t="shared" ref="E50:E60" si="1">C50/SQRT(D50)</f>
+        <f t="shared" ref="E50:E57" si="1">C50/SQRT(D50)</f>
         <v>2.2999999999999998</v>
       </c>
       <c r="F50" s="1"/>
@@ -3104,8 +3083,7 @@
         <v>50</v>
       </c>
       <c r="E59" s="1">
-        <f t="shared" si="1"/>
-        <v>1.697056274847714</v>
+        <v>1.7</v>
       </c>
       <c r="F59" s="1">
         <v>106</v>
@@ -3117,8 +3095,7 @@
         <v>50</v>
       </c>
       <c r="I59" s="7">
-        <f>G59/SQRT(H59)</f>
-        <v>2.8284271247461898</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -3135,8 +3112,7 @@
         <v>50</v>
       </c>
       <c r="E60" s="1">
-        <f t="shared" si="1"/>
-        <v>1.697056274847714</v>
+        <v>1.7</v>
       </c>
       <c r="F60" s="19">
         <v>177</v>
@@ -3148,8 +3124,7 @@
         <v>50</v>
       </c>
       <c r="I60" s="7">
-        <f>G60/SQRT(H60)</f>
-        <v>9.3338095116624267</v>
+        <v>9.33</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -3157,7 +3132,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="19">
-        <v>68.736000000000004</v>
+        <v>68.7</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="19">
@@ -3185,8 +3160,7 @@
         <v>5</v>
       </c>
       <c r="E62" s="1">
-        <f>C62/SQRT(D62)</f>
-        <v>19.901004999748128</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -3207,8 +3181,7 @@
         <v>5</v>
       </c>
       <c r="E63" s="1">
-        <f>C63/SQRT(D63)</f>
-        <v>18.91713508964822</v>
+        <v>18.920000000000002</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -3229,8 +3202,7 @@
         <v>3</v>
       </c>
       <c r="E64" s="1">
-        <f>C64/SQRT(D64)</f>
-        <v>8.1406387955737234</v>
+        <v>8.14</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -3251,8 +3223,7 @@
         <v>3</v>
       </c>
       <c r="E65" s="1">
-        <f>C65/SQRT(D65)</f>
-        <v>7.1014083110323973</v>
+        <v>7.1</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -3273,8 +3244,7 @@
         <v>5</v>
       </c>
       <c r="E66" s="1">
-        <f>C66/SQRT(D66)</f>
-        <v>8.9442719099991592</v>
+        <v>8.9</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -3305,17 +3275,16 @@
         <v>95</v>
       </c>
       <c r="B68" s="1">
-        <v>75.658000000000001</v>
+        <v>76.7</v>
       </c>
       <c r="C68" s="1">
-        <v>10.526</v>
+        <v>10.5</v>
       </c>
       <c r="D68" s="1">
         <v>8</v>
       </c>
       <c r="E68" s="1">
-        <f>C68/SQRT(D68)</f>
-        <v>3.7215029893847995</v>
+        <v>3.71</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -3336,8 +3305,7 @@
         <v>7</v>
       </c>
       <c r="E69" s="1">
-        <f>C69/SQRT(D69)</f>
-        <v>5.3670955167310259</v>
+        <v>5.367</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -3387,7 +3355,7 @@
         <v>98</v>
       </c>
       <c r="B72" s="1">
-        <v>121.05</v>
+        <v>121.1</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1">
@@ -3415,8 +3383,7 @@
         <v>7</v>
       </c>
       <c r="E73" s="1">
-        <f>C73/SQRT(D73)</f>
-        <v>11.792491557887889</v>
+        <v>11.79</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -3466,14 +3433,14 @@
         <v>100</v>
       </c>
       <c r="B76" s="1">
-        <v>84.403000000000006</v>
+        <v>84.4</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1">
         <v>6</v>
       </c>
       <c r="E76" s="1">
-        <v>1.1619999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -3485,12 +3452,12 @@
         <v>101</v>
       </c>
       <c r="B77" s="1">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -3550,8 +3517,7 @@
         <v>5</v>
       </c>
       <c r="E80" s="1">
-        <f>C80/SQRT(D80)</f>
-        <v>2.996331089849718</v>
+        <v>2.996</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -3572,8 +3538,7 @@
         <v>5</v>
       </c>
       <c r="E81" s="1">
-        <f>C81/SQRT(D81)</f>
-        <v>3.3541019662496843</v>
+        <v>3.35</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -3594,8 +3559,7 @@
         <v>13</v>
       </c>
       <c r="E82" s="1">
-        <f>C82/SQRT(D82)</f>
-        <v>6.3790522565901355</v>
+        <v>6.4</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -3701,8 +3665,7 @@
         <v>8</v>
       </c>
       <c r="E88" s="1">
-        <f>C88/SQRT(D88)</f>
-        <v>1.6970562748477138</v>
+        <v>1.7</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -3723,8 +3686,7 @@
         <v>6</v>
       </c>
       <c r="E89" s="8">
-        <f>C89/SQRT(D89)</f>
-        <v>3.1435118365717454</v>
+        <v>3.14</v>
       </c>
       <c r="F89" s="8"/>
       <c r="G89" s="8"/>

</xml_diff>

<commit_message>
update the number of significant digits again (so that # of digits of SE matches with that of mean)
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D522A27-189C-0B43-8B75-1FFFD01A550E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D78F8F-EA6C-A24B-8A74-FBA48BAE7E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22400" windowHeight="22760" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -1431,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C9A479-2AA3-884B-8FF7-FA729F57839B}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1481,7 +1481,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="2">
-        <v>2.5</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="D2" s="2">
         <v>66</v>
@@ -1699,7 +1699,7 @@
         <v>41</v>
       </c>
       <c r="E8" s="7">
-        <v>2.0299999999999998</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1747,13 +1747,13 @@
         <v>40.1</v>
       </c>
       <c r="C11" s="1">
-        <v>0.76</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="D11" s="1">
         <v>94.6</v>
       </c>
       <c r="E11" s="7">
-        <v>4.5999999999999996</v>
+        <v>4.58</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1766,7 +1766,7 @@
         <v>76.400000000000006</v>
       </c>
       <c r="E12" s="7">
-        <v>2.2999999999999998</v>
+        <v>2.25</v>
       </c>
       <c r="I12">
         <f>SQRT((I5+J5)/PI())*2</f>
@@ -1806,13 +1806,13 @@
         <v>42.4</v>
       </c>
       <c r="C14" s="8">
-        <v>1.95</v>
+        <v>1.952</v>
       </c>
       <c r="D14" s="8">
         <v>58.37</v>
       </c>
       <c r="E14" s="9">
-        <v>2.2200000000000002</v>
+        <v>2.2250000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1829,8 +1829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41:H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
delete unused CBM thickness data in lung, nerve, ear, etc
</commit_message>
<xml_diff>
--- a/data/adipose_tissue_parameters.xlsx
+++ b/data/adipose_tissue_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B8AC8-4D06-6745-BA8F-5C634F8CFD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB10F9F-123F-9B40-A09E-908061ECC378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22760" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -270,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C45" authorId="0" shapeId="0" xr:uid="{5B8BC328-C175-1645-944D-85396FC5B1C5}">
+    <comment ref="C40" authorId="0" shapeId="0" xr:uid="{5B8BC328-C175-1645-944D-85396FC5B1C5}">
       <text>
         <r>
           <rPr>
@@ -333,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G45" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
+    <comment ref="G40" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
       <text>
         <r>
           <rPr>
@@ -391,7 +391,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="109">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -471,18 +471,6 @@
     <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Kidney)</t>
   </si>
   <si>
-    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Pulmonary alveolus)</t>
-  </si>
-  <si>
-    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Pancreas)</t>
-  </si>
-  <si>
-    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Choroid)</t>
-  </si>
-  <si>
-    <t>Carlson et al., 2003 (11 mo. FVB mice &amp; Peripheral nerve)</t>
-  </si>
-  <si>
     <t>Williams et al., 2020 (5.5 mo. C57Bl/6 mice &amp; Muscle)</t>
   </si>
   <si>
@@ -546,9 +534,6 @@
     <t>Dosso et al., 1990 (17 mo. Zucker rat &amp; Retina)</t>
   </si>
   <si>
-    <t>Fraselle-Jacobs et al., 1987 (6 mo. Wistar rat &amp; Adipose)</t>
-  </si>
-  <si>
     <t>Cherian et al., 2009 (6 mo. Sprague-Dawley rat &amp; Kidney)</t>
   </si>
   <si>
@@ -696,9 +681,6 @@
     <t>McCaleb et al., 1991 (10.5 mo. Wistar rat &amp; Retina)</t>
   </si>
   <si>
-    <t>Smith et al., 1995 (6 mo. Sprague-Dawley rat &amp; Inner ear)</t>
-  </si>
-  <si>
     <t>Robison et al., 1986 (7 mo. Sprague-Dawley rat &amp; Retina)</t>
   </si>
   <si>
@@ -727,9 +709,6 @@
   </si>
   <si>
     <t>Chakrabarti et al., 1991 (6 mo. BB rat &amp; Muscle)</t>
-  </si>
-  <si>
-    <t>Chakrabarti et al., 1991 (6 mo. BB rat &amp; Endoneurial capillary)</t>
   </si>
   <si>
     <t>Chakrabarti et al., 1991 (6 mo. BB rat &amp; Kidney)</t>
@@ -1510,7 +1489,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1">
         <v>49</v>
@@ -1547,7 +1526,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1613,7 +1592,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B6" s="1">
         <v>49</v>
@@ -1650,7 +1629,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1">
         <v>21</v>
@@ -1687,7 +1666,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1">
         <v>27</v>
@@ -1704,7 +1683,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B9" s="1">
         <v>29</v>
@@ -1827,10 +1806,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:E88"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A86" activeCellId="5" sqref="A77:XFD77 A44:XFD44 A19:XFD19 A21:XFD22 A25:XFD25 A86:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1871,7 +1850,7 @@
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B2" s="21">
         <v>50</v>
@@ -1893,7 +1872,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2">
         <v>59</v>
@@ -1915,7 +1894,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2">
         <v>75</v>
@@ -1937,7 +1916,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2">
         <v>108</v>
@@ -1959,7 +1938,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2">
         <v>154</v>
@@ -1981,7 +1960,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2">
         <v>55</v>
@@ -2002,7 +1981,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B8" s="2">
         <v>77</v>
@@ -2023,7 +2002,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B9" s="2">
         <v>158</v>
@@ -2044,7 +2023,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B10" s="2">
         <v>41</v>
@@ -2065,7 +2044,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2">
         <v>64</v>
@@ -2107,7 +2086,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1">
         <v>56.78</v>
@@ -2129,7 +2108,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1">
         <v>107.53</v>
@@ -2193,7 +2172,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1">
         <v>76.75</v>
@@ -2235,19 +2214,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1">
-        <v>67.989999999999995</v>
+        <v>54.75</v>
       </c>
       <c r="C19" s="1">
-        <v>6.95</v>
+        <v>5</v>
       </c>
       <c r="D19" s="2">
         <v>8</v>
       </c>
       <c r="E19" s="2">
-        <v>2.4569999999999999</v>
+        <v>1.768</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="18"/>
@@ -2256,19 +2235,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1">
-        <v>54.75</v>
+        <v>63.13</v>
       </c>
       <c r="C20" s="1">
-        <v>5</v>
+        <v>5.91</v>
       </c>
       <c r="D20" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E20" s="2">
-        <v>1.768</v>
+        <v>1.706</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="18"/>
@@ -2277,19 +2256,19 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1">
-        <v>103.54</v>
+        <v>56.92</v>
       </c>
       <c r="C21" s="1">
-        <v>16.329999999999998</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="D21" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2">
-        <v>5.7735000000000003</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="18"/>
@@ -2297,127 +2276,121 @@
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>28</v>
+      <c r="A22" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="B22" s="1">
-        <v>78.58</v>
-      </c>
-      <c r="C22" s="1">
-        <v>7.06</v>
-      </c>
-      <c r="D22" s="2">
-        <v>3</v>
-      </c>
-      <c r="E22" s="2">
-        <v>4.0759999999999996</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="7"/>
+        <v>107.6</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
+        <v>31</v>
+      </c>
+      <c r="E22" s="1">
+        <v>5.4820000000000002</v>
+      </c>
+      <c r="F22" s="1">
+        <v>102.7</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1">
+        <v>31</v>
+      </c>
+      <c r="I22" s="7">
+        <v>6.44</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
-        <v>53</v>
+      <c r="A23" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="B23" s="1">
-        <v>63.13</v>
-      </c>
-      <c r="C23" s="1">
-        <v>5.91</v>
-      </c>
-      <c r="D23" s="2">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1.706</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="18"/>
+        <v>224.2</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
-        <v>54</v>
+      <c r="A24" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="B24" s="1">
-        <v>56.92</v>
+        <v>48.5</v>
       </c>
       <c r="C24" s="1">
-        <v>4.0199999999999996</v>
-      </c>
-      <c r="D24" s="2">
-        <v>12</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="18"/>
+        <v>7.31</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2.7629999999999999</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1">
-        <v>58.75</v>
-      </c>
-      <c r="C25" s="1">
-        <v>9.86</v>
-      </c>
-      <c r="D25" s="2">
-        <v>15</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2.5459999999999998</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="18"/>
+        <v>67.03</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
+        <v>4.34</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1">
-        <v>107.6</v>
+        <v>65.790000000000006</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
-        <v>31</v>
-      </c>
-      <c r="E26" s="1">
-        <v>5.4820000000000002</v>
-      </c>
-      <c r="F26" s="1">
-        <v>102.7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E26" s="25">
+        <v>5.56</v>
+      </c>
+      <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1">
-        <v>31</v>
-      </c>
-      <c r="I26" s="7">
-        <v>6.44</v>
-      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1">
-        <v>224.2</v>
+        <v>62.58</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27" s="1">
-        <v>27.7</v>
+        <v>2.7</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -2426,19 +2399,17 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B28" s="1">
-        <v>48.5</v>
-      </c>
-      <c r="C28" s="1">
-        <v>7.31</v>
-      </c>
+        <v>70.11</v>
+      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E28" s="1">
-        <v>2.7629999999999999</v>
+        <v>3.63</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -2447,17 +2418,17 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" s="1">
-        <v>67.03</v>
+        <v>74.94</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1">
         <v>3</v>
       </c>
       <c r="E29" s="1">
-        <v>4.34</v>
+        <v>6.62</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -2466,17 +2437,17 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1">
-        <v>65.790000000000006</v>
+        <v>57.35</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
         <v>3</v>
       </c>
-      <c r="E30" s="25">
-        <v>5.56</v>
+      <c r="E30" s="1">
+        <v>4.33</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2485,17 +2456,17 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1">
-        <v>62.58</v>
+        <v>63.5</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1">
         <v>3</v>
       </c>
       <c r="E31" s="1">
-        <v>2.7</v>
+        <v>4.78</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -2504,17 +2475,17 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32" s="1">
-        <v>70.11</v>
+        <v>58.62</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
         <v>3</v>
       </c>
       <c r="E32" s="1">
-        <v>3.63</v>
+        <v>5.17</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2522,18 +2493,18 @@
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>80</v>
+      <c r="A33" s="23" t="s">
+        <v>79</v>
       </c>
       <c r="B33" s="1">
-        <v>74.94</v>
+        <v>74.23</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1">
         <v>3</v>
       </c>
       <c r="E33" s="1">
-        <v>6.62</v>
+        <v>2.8</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2541,18 +2512,18 @@
       <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>81</v>
+      <c r="A34" s="20" t="s">
+        <v>80</v>
       </c>
       <c r="B34" s="1">
-        <v>57.35</v>
+        <v>97.49</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
         <v>3</v>
       </c>
       <c r="E34" s="1">
-        <v>4.33</v>
+        <v>12.27</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2560,18 +2531,18 @@
       <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>82</v>
+      <c r="A35" s="20" t="s">
+        <v>81</v>
       </c>
       <c r="B35" s="1">
-        <v>63.5</v>
+        <v>109.5</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1">
         <v>3</v>
       </c>
       <c r="E35" s="1">
-        <v>4.78</v>
+        <v>11.93</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2579,18 +2550,18 @@
       <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>83</v>
+      <c r="A36" s="20" t="s">
+        <v>82</v>
       </c>
       <c r="B36" s="1">
-        <v>58.62</v>
+        <v>108.43</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
         <v>3</v>
       </c>
       <c r="E36" s="1">
-        <v>5.17</v>
+        <v>14.51</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -2598,172 +2569,183 @@
       <c r="I36" s="7"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="23" t="s">
-        <v>84</v>
+      <c r="A37" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="B37" s="1">
-        <v>74.23</v>
+        <v>61.87</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E37" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="F37" s="1"/>
+        <v>1.33</v>
+      </c>
+      <c r="F37" s="1">
+        <v>68.13</v>
+      </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="7"/>
+      <c r="H37" s="1">
+        <v>6</v>
+      </c>
+      <c r="I37" s="7">
+        <v>1.66</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
-        <v>85</v>
+      <c r="A38" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="B38" s="1">
-        <v>97.49</v>
+        <v>55.67</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E38" s="1">
-        <v>12.27</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>1.04</v>
+      </c>
+      <c r="F38" s="1">
+        <v>57.82</v>
+      </c>
       <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="7"/>
+      <c r="H38" s="1">
+        <v>7</v>
+      </c>
+      <c r="I38" s="7">
+        <v>1.24</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="20" t="s">
-        <v>86</v>
+      <c r="A39" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="B39" s="1">
-        <v>109.5</v>
-      </c>
-      <c r="C39" s="1"/>
+        <v>93.6</v>
+      </c>
+      <c r="C39" s="1">
+        <v>6.12</v>
+      </c>
       <c r="D39" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E39" s="1">
-        <v>11.93</v>
-      </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="7"/>
+        <v>2.7370000000000001</v>
+      </c>
+      <c r="F39" s="1">
+        <v>104.6</v>
+      </c>
+      <c r="G39" s="1">
+        <v>4.58</v>
+      </c>
+      <c r="H39" s="1">
+        <v>4</v>
+      </c>
+      <c r="I39" s="7">
+        <f>G39/SQRT(H39)</f>
+        <v>2.29</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="20" t="s">
-        <v>87</v>
+      <c r="A40" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B40" s="1">
-        <v>108.43</v>
+        <v>89</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="1">
-        <v>3</v>
-      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="1">
-        <v>14.51</v>
-      </c>
-      <c r="F40" s="1"/>
+        <f>B40*2.2/100</f>
+        <v>1.9580000000000002</v>
+      </c>
+      <c r="F40" s="1">
+        <v>113.4</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="7"/>
+      <c r="I40" s="7">
+        <f>B40*2/100</f>
+        <v>1.78</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B41" s="1">
-        <v>61.87</v>
-      </c>
-      <c r="C41" s="1"/>
+        <v>50.8</v>
+      </c>
+      <c r="C41" s="1">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="D41" s="1">
         <v>6</v>
       </c>
       <c r="E41" s="1">
-        <v>1.33</v>
-      </c>
-      <c r="F41" s="1">
-        <v>68.13</v>
-      </c>
+        <v>2.08</v>
+      </c>
+      <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1">
-        <v>6</v>
-      </c>
-      <c r="I41" s="7">
-        <v>1.66</v>
-      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B42" s="1">
-        <v>55.67</v>
-      </c>
-      <c r="C42" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="C42" s="1">
+        <v>9.9</v>
+      </c>
       <c r="D42" s="1">
         <v>6</v>
       </c>
       <c r="E42" s="1">
-        <v>1.04</v>
-      </c>
-      <c r="F42" s="1">
-        <v>57.82</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1">
-        <v>7</v>
-      </c>
-      <c r="I42" s="7">
-        <v>1.24</v>
-      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B43" s="1">
-        <v>93.6</v>
-      </c>
-      <c r="C43" s="1">
-        <v>6.12</v>
-      </c>
-      <c r="D43" s="1">
-        <v>5</v>
-      </c>
+        <v>235.57</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
       <c r="E43" s="1">
-        <v>2.7370000000000001</v>
-      </c>
-      <c r="F43" s="1">
-        <v>104.6</v>
-      </c>
-      <c r="G43" s="1">
-        <v>4.58</v>
-      </c>
-      <c r="H43" s="1">
-        <v>4</v>
-      </c>
-      <c r="I43" s="7">
-        <f>G43/SQRT(H43)</f>
-        <v>2.29</v>
-      </c>
+        <v>1.05</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B44" s="1">
-        <v>108.8</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="C44" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="D44" s="1">
+        <v>4</v>
+      </c>
       <c r="E44" s="1">
-        <v>11.2</v>
+        <f>C44/SQRT(D44)</f>
+        <v>3.4</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -2772,42 +2754,42 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B45" s="1">
-        <v>89</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+        <v>129.1</v>
+      </c>
+      <c r="C45" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D45" s="1">
+        <v>4</v>
+      </c>
       <c r="E45" s="1">
-        <f>B45*2.2/100</f>
-        <v>1.9580000000000002</v>
-      </c>
-      <c r="F45" s="1">
-        <v>113.4</v>
-      </c>
+        <f t="shared" ref="E45:E52" si="1">C45/SQRT(D45)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="7">
-        <f>B45*2/100</f>
-        <v>1.78</v>
-      </c>
+      <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B46" s="1">
-        <v>50.8</v>
+        <v>135.4</v>
       </c>
       <c r="C46" s="1">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
       <c r="D46" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E46" s="1">
-        <v>2.08</v>
+        <f t="shared" si="1"/>
+        <v>1.75</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -2816,19 +2798,20 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B47" s="1">
-        <v>81</v>
+        <v>147.30000000000001</v>
       </c>
       <c r="C47" s="1">
-        <v>9.9</v>
+        <v>1.3</v>
       </c>
       <c r="D47" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E47" s="1">
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>0.65</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -2837,15 +2820,20 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B48" s="1">
-        <v>235.57</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
+        <v>154.1</v>
+      </c>
+      <c r="C48" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D48" s="1">
+        <v>4</v>
+      </c>
       <c r="E48" s="1">
-        <v>1.05</v>
+        <f t="shared" si="1"/>
+        <v>1.75</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2854,20 +2842,20 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B49" s="1">
-        <v>119</v>
+        <v>160.5</v>
       </c>
       <c r="C49" s="1">
-        <v>6.8</v>
+        <v>3.8</v>
       </c>
       <c r="D49" s="1">
         <v>4</v>
       </c>
       <c r="E49" s="1">
-        <f>C49/SQRT(D49)</f>
-        <v>3.4</v>
+        <f t="shared" si="1"/>
+        <v>1.9</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2876,20 +2864,20 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B50" s="1">
-        <v>129.1</v>
+        <v>184.6</v>
       </c>
       <c r="C50" s="1">
-        <v>4.5999999999999996</v>
+        <v>6.5</v>
       </c>
       <c r="D50" s="1">
         <v>4</v>
       </c>
       <c r="E50" s="1">
-        <f t="shared" ref="E50:E57" si="1">C50/SQRT(D50)</f>
-        <v>2.2999999999999998</v>
+        <f t="shared" si="1"/>
+        <v>3.25</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2897,21 +2885,21 @@
       <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
-        <v>39</v>
+      <c r="A51" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="B51" s="1">
-        <v>135.4</v>
+        <v>205.3</v>
       </c>
       <c r="C51" s="1">
-        <v>3.5</v>
+        <v>7.2</v>
       </c>
       <c r="D51" s="1">
         <v>4</v>
       </c>
       <c r="E51" s="1">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>3.6</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2919,21 +2907,21 @@
       <c r="I51" s="7"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>40</v>
+      <c r="A52" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="B52" s="1">
-        <v>147.30000000000001</v>
+        <v>238.3</v>
       </c>
       <c r="C52" s="1">
-        <v>1.3</v>
+        <v>11.4</v>
       </c>
       <c r="D52" s="1">
         <v>4</v>
       </c>
       <c r="E52" s="1">
         <f t="shared" si="1"/>
-        <v>0.65</v>
+        <v>5.7</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2942,20 +2930,17 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B53" s="1">
-        <v>154.1</v>
-      </c>
-      <c r="C53" s="1">
-        <v>3.5</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="C53" s="1"/>
       <c r="D53" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>10</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -2964,86 +2949,96 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B54" s="1">
-        <v>160.5</v>
+        <v>90</v>
       </c>
       <c r="C54" s="1">
-        <v>3.8</v>
+        <v>12</v>
       </c>
       <c r="D54" s="1">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="7"/>
+        <v>1.7</v>
+      </c>
+      <c r="F54" s="1">
+        <v>106</v>
+      </c>
+      <c r="G54" s="1">
+        <v>20</v>
+      </c>
+      <c r="H54" s="1">
+        <v>50</v>
+      </c>
+      <c r="I54" s="7">
+        <v>2.83</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="19">
+        <v>87</v>
+      </c>
+      <c r="C55" s="19">
+        <v>12</v>
+      </c>
+      <c r="D55" s="19">
+        <v>50</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="F55" s="19">
+        <v>177</v>
+      </c>
+      <c r="G55" s="19">
+        <v>66</v>
+      </c>
+      <c r="H55" s="19">
+        <v>50</v>
+      </c>
+      <c r="I55" s="7">
+        <v>9.33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B55" s="1">
-        <v>184.6</v>
-      </c>
-      <c r="C55" s="1">
-        <v>6.5</v>
-      </c>
-      <c r="D55" s="1">
-        <v>4</v>
-      </c>
-      <c r="E55" s="1">
-        <f t="shared" si="1"/>
-        <v>3.25</v>
-      </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="7"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B56" s="1">
-        <v>205.3</v>
-      </c>
-      <c r="C56" s="1">
-        <v>7.2</v>
-      </c>
-      <c r="D56" s="1">
-        <v>4</v>
-      </c>
-      <c r="E56" s="1">
-        <f t="shared" si="1"/>
-        <v>3.6</v>
-      </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="7"/>
+      <c r="B56" s="19">
+        <v>68.7</v>
+      </c>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19">
+        <v>6</v>
+      </c>
+      <c r="E56" s="19">
+        <v>4.22</v>
+      </c>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="27"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="23" t="s">
-        <v>45</v>
+      <c r="A57" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="B57" s="1">
-        <v>238.3</v>
+        <v>166.7</v>
       </c>
       <c r="C57" s="1">
-        <v>11.4</v>
+        <v>44.5</v>
       </c>
       <c r="D57" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" si="1"/>
-        <v>5.7</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -3052,17 +3047,19 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B58" s="1">
-        <v>305</v>
-      </c>
-      <c r="C58" s="1"/>
+        <v>206.5</v>
+      </c>
+      <c r="C58" s="1">
+        <v>42.3</v>
+      </c>
       <c r="D58" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E58" s="1">
-        <v>10</v>
+        <v>18.920000000000002</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -3071,96 +3068,80 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B59" s="1">
-        <v>90</v>
+        <v>96.7</v>
       </c>
       <c r="C59" s="1">
-        <v>12</v>
+        <v>14.1</v>
       </c>
       <c r="D59" s="1">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E59" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="F59" s="1">
-        <v>106</v>
-      </c>
-      <c r="G59" s="1">
-        <v>20</v>
-      </c>
-      <c r="H59" s="1">
-        <v>50</v>
-      </c>
-      <c r="I59" s="7">
-        <v>2.83</v>
-      </c>
+        <v>8.14</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="7"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B60" s="19">
+        <v>86</v>
+      </c>
+      <c r="B60" s="1">
+        <v>93.9</v>
+      </c>
+      <c r="C60" s="1">
+        <v>12.3</v>
+      </c>
+      <c r="D60" s="1">
+        <v>3</v>
+      </c>
+      <c r="E60" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="7"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C60" s="19">
-        <v>12</v>
-      </c>
-      <c r="D60" s="19">
-        <v>50</v>
-      </c>
-      <c r="E60" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="F60" s="19">
-        <v>177</v>
-      </c>
-      <c r="G60" s="19">
-        <v>66</v>
-      </c>
-      <c r="H60" s="19">
-        <v>50</v>
-      </c>
-      <c r="I60" s="7">
-        <v>9.33</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B61" s="19">
-        <v>68.7</v>
-      </c>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19">
-        <v>6</v>
-      </c>
-      <c r="E61" s="19">
-        <v>4.22</v>
-      </c>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="27"/>
+      <c r="B61" s="1">
+        <v>85</v>
+      </c>
+      <c r="C61" s="1">
+        <v>20</v>
+      </c>
+      <c r="D61" s="1">
+        <v>5</v>
+      </c>
+      <c r="E61" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="7"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B62" s="1">
-        <v>166.7</v>
-      </c>
-      <c r="C62" s="1">
-        <v>44.5</v>
-      </c>
+        <v>66.141999999999996</v>
+      </c>
+      <c r="C62" s="1"/>
       <c r="D62" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E62" s="1">
-        <v>19.899999999999999</v>
+        <v>2.7559999999999998</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -3169,19 +3150,19 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B63" s="1">
-        <v>206.5</v>
+        <v>75.7</v>
       </c>
       <c r="C63" s="1">
-        <v>42.3</v>
+        <v>10.5</v>
       </c>
       <c r="D63" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E63" s="1">
-        <v>18.920000000000002</v>
+        <v>3.72</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -3190,19 +3171,19 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B64" s="1">
-        <v>96.7</v>
+        <v>111.8</v>
       </c>
       <c r="C64" s="1">
-        <v>14.1</v>
+        <v>14.2</v>
       </c>
       <c r="D64" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E64" s="1">
-        <v>8.14</v>
+        <v>5.367</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -3214,16 +3195,14 @@
         <v>91</v>
       </c>
       <c r="B65" s="1">
-        <v>93.9</v>
-      </c>
-      <c r="C65" s="1">
-        <v>12.3</v>
-      </c>
+        <v>81.58</v>
+      </c>
+      <c r="C65" s="1"/>
       <c r="D65" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E65" s="1">
-        <v>7.1</v>
+        <v>7.89</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -3235,16 +3214,14 @@
         <v>92</v>
       </c>
       <c r="B66" s="1">
-        <v>85</v>
-      </c>
-      <c r="C66" s="1">
-        <v>20</v>
-      </c>
+        <v>94.74</v>
+      </c>
+      <c r="C66" s="1"/>
       <c r="D66" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E66" s="1">
-        <v>8.9</v>
+        <v>7.89</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -3252,18 +3229,18 @@
       <c r="I66" s="7"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="11" t="s">
-        <v>94</v>
+      <c r="A67" s="23" t="s">
+        <v>93</v>
       </c>
       <c r="B67" s="1">
-        <v>66.141999999999996</v>
+        <v>121.1</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E67" s="1">
-        <v>2.7559999999999998</v>
+        <v>19.3</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -3272,19 +3249,19 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B68" s="1">
-        <v>75.7</v>
+        <v>160.4</v>
       </c>
       <c r="C68" s="1">
-        <v>10.5</v>
+        <v>31.2</v>
       </c>
       <c r="D68" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E68" s="1">
-        <v>3.72</v>
+        <v>11.79</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -3293,19 +3270,17 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B69" s="1">
-        <v>111.8</v>
-      </c>
-      <c r="C69" s="1">
-        <v>14.2</v>
-      </c>
+        <v>134.6</v>
+      </c>
+      <c r="C69" s="1"/>
       <c r="D69" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E69" s="1">
-        <v>5.367</v>
+        <v>7.7</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -3314,17 +3289,17 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B70" s="1">
-        <v>81.58</v>
+        <v>95.1</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E70" s="1">
-        <v>7.89</v>
+        <v>3.3</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -3333,17 +3308,17 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B71" s="1">
-        <v>94.74</v>
+        <v>84.4</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E71" s="1">
-        <v>7.89</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -3351,18 +3326,21 @@
       <c r="I71" s="7"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="23" t="s">
-        <v>98</v>
+      <c r="A72" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="B72" s="1">
-        <v>121.1</v>
-      </c>
-      <c r="C72" s="1"/>
+        <v>122.9</v>
+      </c>
+      <c r="C72" s="1">
+        <v>19.600000000000001</v>
+      </c>
       <c r="D72" s="1">
         <v>4</v>
       </c>
       <c r="E72" s="1">
-        <v>19.3</v>
+        <f>C72/SQRT(D72)</f>
+        <v>9.8000000000000007</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -3371,19 +3349,15 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B73" s="1">
-        <v>160.4</v>
-      </c>
-      <c r="C73" s="1">
-        <v>31.2</v>
-      </c>
-      <c r="D73" s="1">
-        <v>7</v>
-      </c>
+        <v>79.400000000000006</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
       <c r="E73" s="1">
-        <v>11.79</v>
+        <v>1.9</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -3392,17 +3366,19 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B74" s="1">
-        <v>134.6</v>
-      </c>
-      <c r="C74" s="1"/>
+        <v>146.19999999999999</v>
+      </c>
+      <c r="C74" s="1">
+        <v>6.7</v>
+      </c>
       <c r="D74" s="1">
         <v>5</v>
       </c>
       <c r="E74" s="1">
-        <v>7.7</v>
+        <v>2.996</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -3411,17 +3387,19 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B75" s="1">
-        <v>95.1</v>
-      </c>
-      <c r="C75" s="1"/>
+        <v>97.4</v>
+      </c>
+      <c r="C75" s="1">
+        <v>7.5</v>
+      </c>
       <c r="D75" s="1">
         <v>5</v>
       </c>
       <c r="E75" s="1">
-        <v>3.3</v>
+        <v>3.35</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -3430,17 +3408,19 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B76" s="1">
-        <v>84.4</v>
-      </c>
-      <c r="C76" s="1"/>
+        <v>159</v>
+      </c>
+      <c r="C76" s="1">
+        <v>23</v>
+      </c>
       <c r="D76" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E76" s="1">
-        <v>1.1599999999999999</v>
+        <v>6.38</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -3449,15 +3429,15 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B77" s="1">
-        <v>100</v>
+        <v>161.9</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1">
-        <v>10</v>
+        <v>3.7</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -3466,20 +3446,15 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B78" s="1">
-        <v>122.9</v>
-      </c>
-      <c r="C78" s="1">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="D78" s="1">
-        <v>4</v>
-      </c>
+        <v>142.69999999999999</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
       <c r="E78" s="1">
-        <f>C78/SQRT(D78)</f>
-        <v>9.8000000000000007</v>
+        <v>3.3</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -3487,16 +3462,16 @@
       <c r="I78" s="7"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="11" t="s">
-        <v>103</v>
+      <c r="A79" s="23" t="s">
+        <v>105</v>
       </c>
       <c r="B79" s="1">
-        <v>79.400000000000006</v>
+        <v>125</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1">
-        <v>1.9</v>
+        <v>3.2</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -3504,20 +3479,16 @@
       <c r="I79" s="7"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" s="11" t="s">
-        <v>104</v>
+      <c r="A80" s="23" t="s">
+        <v>106</v>
       </c>
       <c r="B80" s="1">
-        <v>146.19999999999999</v>
-      </c>
-      <c r="C80" s="1">
-        <v>6.7</v>
-      </c>
-      <c r="D80" s="1">
-        <v>5</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
       <c r="E80" s="1">
-        <v>2.996</v>
+        <v>20</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -3525,173 +3496,46 @@
       <c r="I80" s="7"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="23" t="s">
         <v>107</v>
       </c>
       <c r="B81" s="1">
-        <v>97.4</v>
+        <v>51.5</v>
       </c>
       <c r="C81" s="1">
-        <v>7.5</v>
+        <v>4.8</v>
       </c>
       <c r="D81" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E81" s="1">
-        <v>3.35</v>
+        <v>1.7</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="7"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="11" t="s">
+    <row r="82" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B82" s="1">
-        <v>159</v>
-      </c>
-      <c r="C82" s="1">
-        <v>23</v>
-      </c>
-      <c r="D82" s="1">
-        <v>13</v>
-      </c>
-      <c r="E82" s="1">
-        <v>6.38</v>
-      </c>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="7"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B83" s="1">
-        <v>161.9</v>
-      </c>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1">
-        <v>3.7</v>
-      </c>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="7"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B84" s="1">
-        <v>142.69999999999999</v>
-      </c>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1">
-        <v>3.3</v>
-      </c>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="7"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B85" s="1">
-        <v>125</v>
-      </c>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="7"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="B86" s="1">
-        <v>142.80000000000001</v>
-      </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="7"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="B87" s="1">
-        <v>326</v>
-      </c>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1">
-        <v>20</v>
-      </c>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="7"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="B88" s="1">
-        <v>51.5</v>
-      </c>
-      <c r="C88" s="1">
-        <v>4.8</v>
-      </c>
-      <c r="D88" s="1">
-        <v>8</v>
-      </c>
-      <c r="E88" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="7"/>
-    </row>
-    <row r="89" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="B89" s="8">
+      <c r="B82" s="8">
         <v>94.6</v>
       </c>
-      <c r="C89" s="8">
+      <c r="C82" s="8">
         <v>7.7</v>
       </c>
-      <c r="D89" s="8">
+      <c r="D82" s="8">
         <v>6</v>
       </c>
-      <c r="E89" s="8">
+      <c r="E82" s="8">
         <v>3.14</v>
       </c>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="9"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>